<commit_message>
obsidian backup auto: 2025-02-01 22:06:41
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/work/QCELLs offboarding/attachments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="776" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E04674AF-6919-4155-B0CA-22C1AA887C81}"/>
+  <xr:revisionPtr revIDLastSave="783" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5866F056-7719-4596-98BB-FE0CE299B2E0}"/>
   <bookViews>
-    <workbookView xWindow="-21697" yWindow="1747" windowWidth="21795" windowHeight="14595" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="1612" yWindow="2782" windowWidth="16201" windowHeight="10576" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="330">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1043,6 +1043,18 @@
   </si>
   <si>
     <t>https://mail.google.com/mail/u/0/#inbox/FMfcgzQZSsGSGPjhgTNRFJZqbgrQjfdK</t>
+  </si>
+  <si>
+    <t>Algorithm Developer V</t>
+  </si>
+  <si>
+    <t>Time Series work, recruiter contact, don't know firm yet</t>
+  </si>
+  <si>
+    <t>Crystal Equation Corporation (Akash Sheth)</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/messaging/thread/2-OGZmMWYxOWUtYTIxMS00ZDI3LWEyZGQtZWUxMTY4ODY2MjcwXzAxMA==/</t>
   </si>
 </sst>
 </file>
@@ -3546,10 +3558,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4387,11 +4395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5994,6 +6002,23 @@
       </c>
       <c r="F89" t="s">
         <v>321</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A90" s="3">
+        <v>45688</v>
+      </c>
+      <c r="B90" t="s">
+        <v>328</v>
+      </c>
+      <c r="C90" t="s">
+        <v>326</v>
+      </c>
+      <c r="D90" t="s">
+        <v>327</v>
+      </c>
+      <c r="F90" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-02-01 22:21:32
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="783" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5866F056-7719-4596-98BB-FE0CE299B2E0}"/>
+  <xr:revisionPtr revIDLastSave="791" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E498B58-F854-4C09-A81C-6DD10D11F9D8}"/>
   <bookViews>
-    <workbookView xWindow="1612" yWindow="2782" windowWidth="16201" windowHeight="10576" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="14016" yWindow="11304" windowWidth="28560" windowHeight="10572" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="333">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1054,14 +1054,23 @@
     <t>Crystal Equation Corporation (Akash Sheth)</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/messaging/thread/2-OGZmMWYxOWUtYTIxMS00ZDI3LWEyZGQtZWUxMTY4ODY2MjcwXzAxMA==/</t>
+    <t>Snap, Inc</t>
+  </si>
+  <si>
+    <t>Something w/ cameras, but not image proc, Seattle</t>
+  </si>
+  <si>
+    <t>web: https://www.linkedin.com/messaging/thread/2-OGZmMWYxOWUtYTIxMS00ZDI3LWEyZGQtZWUxMTY4ODY2MjcwXzAxMA==/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.linkedin.com/jobs/view/4121944870/?trackingId=GN5BZH04NvnkRvk0CRZ9nw%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D02b6f6c3...2706a733%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=14G-2AdlMN7rE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m6n00qp1~2k-null-null&amp;eid=1j75g-m6n00qp1-2k&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUyNDIxOGU0YjU4YWNhZDE0Mjk5YTQ4NzZmNzdjMTAwNmU0NzViNTZmNjg5ZDM4MWEwNzFkOWI5MGQ5N2U1NDlhYjQ2MDliNTU5YTU0NjFjMWRlZTgxODYsMSwx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1147,6 +1156,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1181,7 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1202,6 +1217,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4395,11 +4411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6018,7 +6034,24 @@
         <v>327</v>
       </c>
       <c r="F90" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A91" s="3">
+        <v>45689</v>
+      </c>
+      <c r="B91" t="s">
         <v>329</v>
+      </c>
+      <c r="C91" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D91" t="s">
+        <v>330</v>
+      </c>
+      <c r="F91" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-02-01 22:41:34
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="791" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E498B58-F854-4C09-A81C-6DD10D11F9D8}"/>
+  <xr:revisionPtr revIDLastSave="797" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47C1B85C-C62E-4F4A-A07C-0ADCE08AE6AD}"/>
   <bookViews>
     <workbookView xWindow="14016" yWindow="11304" windowWidth="28560" windowHeight="10572" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="337">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1064,6 +1064,18 @@
   </si>
   <si>
     <t xml:space="preserve"> https://www.linkedin.com/jobs/view/4121944870/?trackingId=GN5BZH04NvnkRvk0CRZ9nw%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D02b6f6c3...2706a733%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=14G-2AdlMN7rE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m6n00qp1~2k-null-null&amp;eid=1j75g-m6n00qp1-2k&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUyNDIxOGU0YjU4YWNhZDE0Mjk5YTQ4NzZmNzdjMTAwNmU0NzViNTZmNjg5ZDM4MWEwNzFkOWI5MGQ5N2U1NDlhYjQ2MDliNTU5YTU0NjFjMWRlZTgxODYsMSwx</t>
+  </si>
+  <si>
+    <t>Blue Cross Blue Shield</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist - Behavioral Health</t>
+  </si>
+  <si>
+    <t>Eagan, MN.  I've got everything but NLP and modern MLOPS</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4133418512/?trackingId=qPpRJCq9tIYrZge8%2BTfiKg%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D600f2bcc...51656825%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=3jbgn2Vlws4HE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m6k6pmao~zu-null-null&amp;eid=1j75g-m6k6pmao-zu&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUyNDQxN2U1YmQ4ZmM2ZDA0ODk5YTQ4NzZmNzdjMTAwNmU0NzViNTZhMTkxODk4ZDg5N2JmNGUwMzU3MDZjMzBlYzQwZTQ3ODZlNmRiNzc0Nzk5YTNjYWIsMSwx</t>
   </si>
 </sst>
 </file>
@@ -4411,11 +4423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6052,6 +6064,23 @@
       </c>
       <c r="F91" t="s">
         <v>332</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A92" s="3">
+        <v>45689</v>
+      </c>
+      <c r="B92" t="s">
+        <v>333</v>
+      </c>
+      <c r="C92" t="s">
+        <v>334</v>
+      </c>
+      <c r="D92" t="s">
+        <v>335</v>
+      </c>
+      <c r="F92" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-02-01 22:55:18
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
refwrangle/refwrangle.py
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="797" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47C1B85C-C62E-4F4A-A07C-0ADCE08AE6AD}"/>
+  <xr:revisionPtr revIDLastSave="807" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C36EE9D-5AF7-4FB7-8EF0-E5CA1EC42CB1}"/>
   <bookViews>
-    <workbookView xWindow="14016" yWindow="11304" windowWidth="28560" windowHeight="10572" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="14016" yWindow="11304" windowWidth="28560" windowHeight="10572" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="343">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1076,13 +1076,31 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/4133418512/?trackingId=qPpRJCq9tIYrZge8%2BTfiKg%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D600f2bcc...51656825%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=3jbgn2Vlws4HE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m6k6pmao~zu-null-null&amp;eid=1j75g-m6k6pmao-zu&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUyNDQxN2U1YmQ4ZmM2ZDA0ODk5YTQ4NzZmNzdjMTAwNmU0NzViNTZhMTkxODk4ZDg5N2JmNGUwMzU3MDZjMzBlYzQwZTQ3ODZlNmRiNzc0Nzk5YTNjYWIsMSwx</t>
+  </si>
+  <si>
+    <t>LTIMindtree</t>
+  </si>
+  <si>
+    <t>Milwaukee, looks like I could do it right away</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4136189546/?refId=XoCq6J7kSHqOS08qN0uC9w%3D%3D&amp;trackingId=%2Fy21%2Bq3PRRuIo%2FFpZmVQyw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/0/#inbox/FMfcgzQZSsPVcBnsRvfJSxcKdrgTJWQd</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/0/#inbox/FMfcgzQZSsPVbzhGKvNxBLlNnhrvKhQZ</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/0/#inbox/FMfcgzQZSsPVbxXgzxPqdsJWwjgqRbbg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1168,12 +1186,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1208,7 +1220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1229,7 +1241,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4423,11 +4434,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A93" sqref="A93"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6056,7 +6067,7 @@
       <c r="B91" t="s">
         <v>329</v>
       </c>
-      <c r="C91" s="16" t="s">
+      <c r="C91" t="s">
         <v>61</v>
       </c>
       <c r="D91" t="s">
@@ -6064,6 +6075,9 @@
       </c>
       <c r="F91" t="s">
         <v>332</v>
+      </c>
+      <c r="G91" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.45">
@@ -6081,6 +6095,29 @@
       </c>
       <c r="F92" t="s">
         <v>336</v>
+      </c>
+      <c r="G92" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A93" s="3">
+        <v>45689</v>
+      </c>
+      <c r="B93" t="s">
+        <v>337</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" t="s">
+        <v>338</v>
+      </c>
+      <c r="F93" t="s">
+        <v>339</v>
+      </c>
+      <c r="G93" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ignore a bunch of stuff
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="835" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E688471A-46D6-4EFD-8943-7488C4102EA0}"/>
+  <xr:revisionPtr revIDLastSave="855" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{426262C9-72C6-4049-A648-C05133FA3618}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8" yWindow="8" windowWidth="21585" windowHeight="14385" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="-21697" yWindow="1747" windowWidth="21795" windowHeight="14595" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="370">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1136,6 +1136,45 @@
   </si>
   <si>
     <t>Not sure</t>
+  </si>
+  <si>
+    <t>LatentView Analytics</t>
+  </si>
+  <si>
+    <t>Market analyytics, but seattle, easy</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4139907275/?refId=ByteString(length%3D16%2Cbytes%3D150983f7...8f6a262d)&amp;trackingId=JQaQxdwWX0sVJpgbRDE9zw%3D%3D</t>
+  </si>
+  <si>
+    <t>Tata Consultancy Services</t>
+  </si>
+  <si>
+    <t>they want SQL… consulting</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4149289471/?refId=ByteString(length%3D16%2Cbytes%3Da77c4f9b...24e62942)&amp;trackingId=fZD94CNeR4eK%2F1ctw%2B1IBg%3D%3D</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist </t>
+  </si>
+  <si>
+    <t>GLX ANALYTIX</t>
+  </si>
+  <si>
+    <t>Denmark, personalized medicine</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4150250844/?refId=ByteString(length%3D16%2Cbytes%3Db8b66b1f...f79b0827)&amp;trackingId=IJSdoryuUWCZ8UQNmm2Csw%3D%3D</t>
+  </si>
+  <si>
+    <t>SureCost</t>
+  </si>
+  <si>
+    <t>St. Petersburg, Fl,  pharmacy inventory, more of MLOPS?</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4152258208/?refId=I3ESEstkRIyQ0GNGtFx%2FYQ%3D%3D&amp;trackingId=jyT38KXWQ46%2FKZ%2BxwTqcfQ%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -4480,11 +4519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
+      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6238,6 +6277,74 @@
       </c>
       <c r="F97" t="s">
         <v>354</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>45703</v>
+      </c>
+      <c r="B98" t="s">
+        <v>357</v>
+      </c>
+      <c r="C98" t="s">
+        <v>61</v>
+      </c>
+      <c r="D98" t="s">
+        <v>358</v>
+      </c>
+      <c r="F98" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="3">
+        <v>45703</v>
+      </c>
+      <c r="B99" t="s">
+        <v>360</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>361</v>
+      </c>
+      <c r="F99" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="3">
+        <v>45703</v>
+      </c>
+      <c r="B100" t="s">
+        <v>364</v>
+      </c>
+      <c r="C100" t="s">
+        <v>363</v>
+      </c>
+      <c r="D100" t="s">
+        <v>365</v>
+      </c>
+      <c r="F100" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="3">
+        <v>45703</v>
+      </c>
+      <c r="B101" t="s">
+        <v>367</v>
+      </c>
+      <c r="C101" t="s">
+        <v>61</v>
+      </c>
+      <c r="D101" t="s">
+        <v>368</v>
+      </c>
+      <c r="F101" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-02-21 14:10:55
Affected files:
obsidian/Obsidian Share Vault/.obsidian/workspace.json
obsidian/Obsidian Share Vault/Politics/Political Causality/US Elections 2024.md
obsidian/Obsidian Share Vault/Work/Between Jobs/Interview Prep/Basic Math/attachments/Basic Hypothesis Tests.html
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Evans24techSplinterCulturalCtrl.md
obsidian/Obsidian Share Vault/lit/lit_notes/Rampell25genZmenLoveTrump.md
obsidian/Obsidian Share Vault/lit/refwrangle/Perplexity Parsing.md
refwrangle/test/tmp_wkhtmltopdf.pdf
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="855" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{426262C9-72C6-4049-A648-C05133FA3618}"/>
   <bookViews>
-    <workbookView xWindow="-21697" yWindow="1747" windowWidth="21795" windowHeight="14595" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="3375" yWindow="3375" windowWidth="16200" windowHeight="10515" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4522,29 +4522,29 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F101" sqref="F101"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="29.19921875" customWidth="1"/>
+    <col min="4" max="4" width="46.796875" customWidth="1"/>
+    <col min="5" max="5" width="8.53125" customWidth="1"/>
+    <col min="6" max="6" width="28.19921875" customWidth="1"/>
+    <col min="7" max="7" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4564,7 +4564,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>45523</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>45525</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>45528</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>45530</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>45531</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>45534</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>45539</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>45539</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>45539</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>45540</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>45541</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>45541</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>45543</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>45547</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>45548</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>45549</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>45555</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>45555</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>45555</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
         <v>45555</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>45562</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
         <v>45563</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
         <v>45563</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
         <v>45563</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
         <v>45563</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="3">
         <v>45563</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="3">
         <v>45563</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="3">
         <v>45566</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>45569</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="3">
         <v>45570</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>45577</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="3">
         <v>45577</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="3">
         <v>45577</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="3">
         <v>45591</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="3">
         <v>45591</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="3">
         <v>45591</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="3">
         <v>45595</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="3">
         <v>45598</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="3">
         <v>45598</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="3">
         <v>45600</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="3">
         <v>45600</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="3">
         <v>45605</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="3">
         <v>45612</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="3">
         <v>45612</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="3">
         <v>45612</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="13">
         <v>45616</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="3">
         <v>45619</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="3">
         <v>45619</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="3">
         <v>45619</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="3">
         <v>45626</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="3">
         <v>45626</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="3">
         <v>45626</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="3">
         <v>45633</v>
       </c>
@@ -5554,7 +5554,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="3">
         <v>45633</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>45633</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>45635</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>45640</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="3">
         <v>45640</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="3">
         <v>45640</v>
       </c>
@@ -5659,7 +5659,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="3">
         <v>45641</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="3">
         <v>45647</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="3">
         <v>45647</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="3">
         <v>45647</v>
       </c>
@@ -5730,7 +5730,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="3">
         <v>45647</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="3">
         <v>45651</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="3">
         <v>45651</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="3">
         <v>45654</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="3">
         <v>45654</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="3">
         <v>45654</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="3">
         <v>45661</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="3">
         <v>45661</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="3">
         <v>45661</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="3">
         <v>45667</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="3">
         <v>45668</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="3">
         <v>45668</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="3">
         <v>45668</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="3">
         <v>45668</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="3">
         <v>45674</v>
       </c>
@@ -6009,7 +6009,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="3">
         <v>45674</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="3">
         <v>45675</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="3">
         <v>45682</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="3">
         <v>45682</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="3">
         <v>45682</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="3">
         <v>45682</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="3">
         <v>45316</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="3">
         <v>45688</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="3">
         <v>45689</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="3">
         <v>45689</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="3">
         <v>45689</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="3">
         <v>45696</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="3">
         <v>45696</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="3">
         <v>45696</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="3">
         <v>45696</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="3">
         <v>45703</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="3">
         <v>45703</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="3">
         <v>45703</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="3">
         <v>45703</v>
       </c>
@@ -6369,22 +6369,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45539</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45539</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45539</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45540</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45541</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45541</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45543</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45547</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C22" s="3">
         <v>45548</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C23" s="3">
         <v>45549</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C24" s="3">
         <v>45555</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C25" s="3">
         <v>45555</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C26" s="3">
         <v>45555</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C27" s="3">
         <v>45555</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>82</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C29" s="3">
         <v>45563</v>
       </c>
@@ -6807,7 +6807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C30" s="3">
         <v>45563</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C31" s="3">
         <v>45563</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C32" s="3">
         <v>45563</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C33" s="3">
         <v>45563</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C34" s="3">
         <v>45563</v>
       </c>
@@ -6903,23 +6903,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C4" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C5" cm="1">
         <f t="array" ref="C5">IF(SUM(ISERROR(Sheet2!$C$7:$H$34)*1)&gt;0,NA(),COUNTA(_xlfn.UNIQUE(Sheet2!$C$7:$C$34)))</f>
         <v>17</v>
@@ -6936,19 +6936,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -6964,7 +6964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7004,7 +7004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>119</v>
       </c>
@@ -7112,19 +7112,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7220,7 +7220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7244,7 +7244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7260,7 +7260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-01 22:35:51
Affected files:
obsidian/Obsidian Share Vault/.obsidian/workspace.json
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
refwrangle/link_ai_lit.py
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="877" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E56D7EF-73CB-4BA3-B6EF-070B5FDE1C65}"/>
+  <xr:revisionPtr revIDLastSave="888" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03B2B7A5-E7A3-433D-8BA3-55DDE444EC2E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="387">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1211,6 +1211,21 @@
   </si>
   <si>
     <t xml:space="preserve"> https://www.linkedin.com/jobs/view/4099126068/?eBP=CwEAAAGUV6Cr55I-WxahczdbWk5CNtliLU0CyCr3OJLZsRwh9dLddDn5a4M07y39ujVq3zU3jJqPhvtnMvbuX1561MteRZreIa-pCbFSDa_xR4z_y7gpgs0g_fE1aH-iea7_ijshfM_96iDQu6w-VqBZB8MqZmQs3ZNfXOrciVahyDM__ZYGZ4K78EgR6tfmu8a7muTDIRIemLElzm87j-mr9AeLWaw3WnZw81fYoxhboMIQul6uyUVW7SjcEYyxodiC1a-m-zuRIWWeiWC1F15gpyiV6zSs0xgSVuJRMeeUcqTclu0-Uyw87VGp9Dae8VZ_k3jEnkgj6FWgnlf7saHjlDsWPlu_YA6HkOuf3V49NclYqRDuZQLfbyG-ZfpmVERD7STPYOlvmjKVxMI-gpEoqQyUN1f15xTml8K7EXPFpHzjqDyopRTblrTSWvyQCruNg5jZZQ0_dW04IO8vKALtumJgW7yJWc_VFcsO5G8cgQcVp7v9xTvvO_eWbVwuCXM&amp;refId=AE0hxPRAc80zaaxhlr24mg%3D%3D&amp;trackingId=zjXOB5tiGtVc92vsaSG1uw%3D%3D</t>
+  </si>
+  <si>
+    <t>Set up interview for the coming  week</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/0/#inbox/FMfcgzQZTVqLmWTqjNVQCzZbntHZsRJL</t>
+  </si>
+  <si>
+    <t>Radley James</t>
+  </si>
+  <si>
+    <t>Biz stuff, I think, Seattle</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4157165676/?refId=ByteString(length%3D16%2Cbytes%3D25e4c5dd...c3390254)&amp;trackingId=4WGOAiRiIgmaF6PjHt1tGg%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -4555,11 +4570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D99" sqref="D99"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6438,6 +6453,40 @@
       </c>
       <c r="F104" t="s">
         <v>380</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A105" s="3">
+        <v>45717</v>
+      </c>
+      <c r="B105" t="s">
+        <v>287</v>
+      </c>
+      <c r="C105" t="s">
+        <v>93</v>
+      </c>
+      <c r="D105" t="s">
+        <v>382</v>
+      </c>
+      <c r="F105" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A106" s="3">
+        <v>45717</v>
+      </c>
+      <c r="B106" t="s">
+        <v>384</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" t="s">
+        <v>385</v>
+      </c>
+      <c r="F106" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-02 10:37:00
Affected files:
obsidian/Obsidian Share Vault/.obsidian/workspace.json
obsidian/Obsidian Share Vault/.smart-env/multi/work_Between_Jobs_Interview_Prep_SQL_training_SQL_for_Data_Science_(Coursera,_UC-Davis)_Module_2_-_SQL_for_Data_Science_md.ajson
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
refwrangle/link_ai_lit.py
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="888" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03B2B7A5-E7A3-433D-8BA3-55DDE444EC2E}"/>
+  <xr:revisionPtr revIDLastSave="903" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE27C318-CFBC-4280-9DAB-168CE9CAC96A}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="-19395" yWindow="4050" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="394">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1226,6 +1226,27 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/4157165676/?refId=ByteString(length%3D16%2Cbytes%3D25e4c5dd...c3390254)&amp;trackingId=4WGOAiRiIgmaF6PjHt1tGg%3D%3D</t>
+  </si>
+  <si>
+    <t>Blue Origin</t>
+  </si>
+  <si>
+    <t>Rockets! Seattle</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4129694097/?trackingId=38dxlXxhCYugQX9ivFet9Q%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3Dc5d4aa82...11ce833a%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=2rQToEMrxErbE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m774gzwn~6v-null-null&amp;eid=1j75g-m774gzwn-6v&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUzNDAxOWVlYmM4OWNmZDM0NDkxYTQ4NzZmNzdjMTAwNmU0NzViNTZiNDg3OGE5MjhhNDdjOGY4MzJmYmZlY2I5MjViZTU0ZDJiMWZjNDg2N2FlNjJjOWIsMSwx</t>
+  </si>
+  <si>
+    <t>Wex</t>
+  </si>
+  <si>
+    <t>Risk Data Scientist - Risk Solutions (R17002)</t>
+  </si>
+  <si>
+    <t>Financial risk, but in Seattle or remote</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4127911752/?trackingId=P1ghrR8o3oaZGoDaeLKXiA%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D8d299bb8...ead4a064%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=1JijpxNTFgpHE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m75kqt9z~7h-null-null&amp;eid=1j75g-m75kqt9z-7h&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUzNDMxNmUxYjY4OWM4ZDg0NzlhYTQ4NzZmNzdjMTAwNmU0NzViNTZmNDhjODZiM2I5MTNkYWQxMWQxYjUyMmQ3NzUwNTA4ZGMzZWE4Y2UzNTZjYWFlNjEsMSwx</t>
   </si>
 </sst>
 </file>
@@ -4570,32 +4591,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <selection pane="bottomLeft" activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" customWidth="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="29.19921875" customWidth="1"/>
-    <col min="4" max="4" width="46.796875" customWidth="1"/>
-    <col min="5" max="5" width="8.53125" customWidth="1"/>
-    <col min="6" max="6" width="28.19921875" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4615,7 +4636,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45523</v>
       </c>
@@ -4629,7 +4650,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45525</v>
       </c>
@@ -4646,7 +4667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>45528</v>
       </c>
@@ -4666,7 +4687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>45530</v>
       </c>
@@ -4683,7 +4704,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>45531</v>
       </c>
@@ -4700,7 +4721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>45534</v>
       </c>
@@ -4714,7 +4735,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4731,7 +4752,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45539</v>
       </c>
@@ -4751,7 +4772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45539</v>
       </c>
@@ -4769,7 +4790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>45539</v>
       </c>
@@ -4786,7 +4807,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>45540</v>
       </c>
@@ -4806,7 +4827,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>45541</v>
       </c>
@@ -4826,7 +4847,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>45541</v>
       </c>
@@ -4846,7 +4867,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>45543</v>
       </c>
@@ -4866,7 +4887,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>45547</v>
       </c>
@@ -4883,7 +4904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>45548</v>
       </c>
@@ -4900,7 +4921,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>45549</v>
       </c>
@@ -4917,7 +4938,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45555</v>
       </c>
@@ -4937,7 +4958,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>45555</v>
       </c>
@@ -4954,7 +4975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>45555</v>
       </c>
@@ -4971,7 +4992,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>45555</v>
       </c>
@@ -4988,7 +5009,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>45562</v>
       </c>
@@ -5005,7 +5026,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>45563</v>
       </c>
@@ -5022,7 +5043,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>45563</v>
       </c>
@@ -5039,7 +5060,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>45563</v>
       </c>
@@ -5056,7 +5077,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>45563</v>
       </c>
@@ -5073,7 +5094,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45563</v>
       </c>
@@ -5093,7 +5114,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>45563</v>
       </c>
@@ -5110,7 +5131,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>45566</v>
       </c>
@@ -5127,7 +5148,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>45569</v>
       </c>
@@ -5144,7 +5165,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>45570</v>
       </c>
@@ -5161,7 +5182,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>45577</v>
       </c>
@@ -5181,7 +5202,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>45577</v>
       </c>
@@ -5201,7 +5222,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>45577</v>
       </c>
@@ -5218,7 +5239,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>45591</v>
       </c>
@@ -5238,7 +5259,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>45591</v>
       </c>
@@ -5255,7 +5276,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>45591</v>
       </c>
@@ -5275,7 +5296,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>45595</v>
       </c>
@@ -5292,7 +5313,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>45598</v>
       </c>
@@ -5309,7 +5330,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>45598</v>
       </c>
@@ -5329,7 +5350,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>45600</v>
       </c>
@@ -5346,7 +5367,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>45600</v>
       </c>
@@ -5363,7 +5384,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>45605</v>
       </c>
@@ -5383,7 +5404,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -5403,7 +5424,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45612</v>
       </c>
@@ -5420,7 +5441,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>45612</v>
       </c>
@@ -5440,7 +5461,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>45612</v>
       </c>
@@ -5457,7 +5478,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>45616</v>
       </c>
@@ -5474,7 +5495,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>45619</v>
       </c>
@@ -5491,7 +5512,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>45619</v>
       </c>
@@ -5508,7 +5529,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>45619</v>
       </c>
@@ -5528,7 +5549,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>45626</v>
       </c>
@@ -5548,7 +5569,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>45626</v>
       </c>
@@ -5568,7 +5589,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>45626</v>
       </c>
@@ -5588,7 +5609,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>45633</v>
       </c>
@@ -5605,7 +5626,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>45633</v>
       </c>
@@ -5622,7 +5643,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>45633</v>
       </c>
@@ -5639,7 +5660,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>45635</v>
       </c>
@@ -5656,7 +5677,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>45640</v>
       </c>
@@ -5676,7 +5697,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>45640</v>
       </c>
@@ -5693,7 +5714,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>45640</v>
       </c>
@@ -5710,7 +5731,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>45641</v>
       </c>
@@ -5727,7 +5748,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>45647</v>
       </c>
@@ -5747,7 +5768,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>45647</v>
       </c>
@@ -5764,7 +5785,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>45647</v>
       </c>
@@ -5781,7 +5802,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>45647</v>
       </c>
@@ -5801,7 +5822,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>45651</v>
       </c>
@@ -5818,7 +5839,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>45651</v>
       </c>
@@ -5838,7 +5859,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>45654</v>
       </c>
@@ -5855,7 +5876,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>45654</v>
       </c>
@@ -5872,7 +5893,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>45654</v>
       </c>
@@ -5889,7 +5910,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>45661</v>
       </c>
@@ -5909,7 +5930,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>45661</v>
       </c>
@@ -5926,7 +5947,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>45661</v>
       </c>
@@ -5946,7 +5967,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>45667</v>
       </c>
@@ -5966,7 +5987,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>45668</v>
       </c>
@@ -5986,7 +6007,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>45668</v>
       </c>
@@ -6006,7 +6027,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>45668</v>
       </c>
@@ -6023,7 +6044,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>45668</v>
       </c>
@@ -6040,7 +6061,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>45674</v>
       </c>
@@ -6060,7 +6081,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>45674</v>
       </c>
@@ -6077,7 +6098,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>45675</v>
       </c>
@@ -6094,7 +6115,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>45682</v>
       </c>
@@ -6111,7 +6132,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>45682</v>
       </c>
@@ -6128,7 +6149,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>45682</v>
       </c>
@@ -6148,7 +6169,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>45682</v>
       </c>
@@ -6165,7 +6186,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>45316</v>
       </c>
@@ -6182,7 +6203,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>45688</v>
       </c>
@@ -6199,7 +6220,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>45689</v>
       </c>
@@ -6219,7 +6240,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>45689</v>
       </c>
@@ -6239,7 +6260,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>45689</v>
       </c>
@@ -6262,7 +6283,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>45696</v>
       </c>
@@ -6279,7 +6300,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>45696</v>
       </c>
@@ -6296,7 +6317,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>45696</v>
       </c>
@@ -6313,7 +6334,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>45696</v>
       </c>
@@ -6330,7 +6351,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>45703</v>
       </c>
@@ -6347,7 +6368,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>45703</v>
       </c>
@@ -6364,7 +6385,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>45703</v>
       </c>
@@ -6381,7 +6402,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>45703</v>
       </c>
@@ -6398,7 +6419,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>45708</v>
       </c>
@@ -6418,7 +6439,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>45710</v>
       </c>
@@ -6438,7 +6459,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>377</v>
       </c>
@@ -6455,7 +6476,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>45717</v>
       </c>
@@ -6472,7 +6493,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>45717</v>
       </c>
@@ -6487,6 +6508,40 @@
       </c>
       <c r="F106" t="s">
         <v>386</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="3">
+        <v>45717</v>
+      </c>
+      <c r="B107" t="s">
+        <v>387</v>
+      </c>
+      <c r="C107" t="s">
+        <v>70</v>
+      </c>
+      <c r="D107" t="s">
+        <v>388</v>
+      </c>
+      <c r="F107" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="3">
+        <v>45717</v>
+      </c>
+      <c r="B108" t="s">
+        <v>390</v>
+      </c>
+      <c r="C108" t="s">
+        <v>391</v>
+      </c>
+      <c r="D108" t="s">
+        <v>392</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -6499,9 +6554,10 @@
     <hyperlink ref="C21" r:id="rId6" display="https://relx.wd3.myworkdayjobs.com/en-US/RiskSolutions/job/Data-Scientist-III_R81901" xr:uid="{2ADFB246-5260-44CC-A8D4-BBF94451FB42}"/>
     <hyperlink ref="F45" r:id="rId7" location="inbox/FMfcgzQXKDXgdHgsSqKhNMLXNZQBTfTq" xr:uid="{EFC332EF-EC04-4994-B0D6-C5A052113B8F}"/>
     <hyperlink ref="F54" r:id="rId8" location="inbox/FMfcgzQXKWfCxmBwDTCtjNzGrjXrLSGg" xr:uid="{F90DEC25-488D-4CD6-9855-7FF777FB5AF2}"/>
+    <hyperlink ref="F108" r:id="rId9" display="https://www.linkedin.com/jobs/view/4127911752/?trackingId=P1ghrR8o3oaZGoDaeLKXiA%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D8d299bb8...ead4a064%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=1JijpxNTFgpHE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m75kqt9z~7h-null-null&amp;eid=1j75g-m75kqt9z-7h&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUzNDMxNmUxYjY4OWM4ZDg0NzlhYTQ4NzZmNzdjMTAwNmU0NzViNTZmNDhjODZiM2I5MTNkYWQxMWQxYjUyMmQ3NzUwNTA4ZGMzZWE4Y2UzNTZjYWFlNjEsMSwx" xr:uid="{96425F70-4035-4136-B80B-46A73A07E3FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="4294967295" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="4294967295" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -6511,22 +6567,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -6546,7 +6602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -6560,7 +6616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -6577,7 +6633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -6597,7 +6653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -6614,7 +6670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -6631,7 +6687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -6645,7 +6701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -6662,7 +6718,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45539</v>
       </c>
@@ -6682,7 +6738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45539</v>
       </c>
@@ -6699,7 +6755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45539</v>
       </c>
@@ -6716,7 +6772,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45540</v>
       </c>
@@ -6736,7 +6792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45541</v>
       </c>
@@ -6753,7 +6809,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45541</v>
       </c>
@@ -6773,7 +6829,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45543</v>
       </c>
@@ -6793,7 +6849,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45547</v>
       </c>
@@ -6810,7 +6866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>45548</v>
       </c>
@@ -6827,7 +6883,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>45549</v>
       </c>
@@ -6844,7 +6900,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>45555</v>
       </c>
@@ -6864,7 +6920,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>45555</v>
       </c>
@@ -6881,7 +6937,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>45555</v>
       </c>
@@ -6898,7 +6954,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" s="3">
         <v>45555</v>
       </c>
@@ -6915,7 +6971,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>82</v>
       </c>
@@ -6932,7 +6988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>45563</v>
       </c>
@@ -6949,7 +7005,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>45563</v>
       </c>
@@ -6966,7 +7022,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
         <v>45563</v>
       </c>
@@ -6983,7 +7039,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>45563</v>
       </c>
@@ -7000,7 +7056,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C33" s="3">
         <v>45563</v>
       </c>
@@ -7017,7 +7073,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
         <v>45563</v>
       </c>
@@ -7045,23 +7101,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C5" cm="1">
         <f t="array" ref="C5">IF(SUM(ISERROR(Sheet2!$C$7:$H$34)*1)&gt;0,NA(),COUNTA(_xlfn.UNIQUE(Sheet2!$C$7:$C$34)))</f>
         <v>17</v>
@@ -7078,19 +7134,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7098,7 +7154,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7106,7 +7162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7114,7 +7170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7122,7 +7178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7130,7 +7186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7138,7 +7194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7146,7 +7202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7154,7 +7210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7162,7 +7218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7170,7 +7226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7178,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7186,7 +7242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7194,7 +7250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7202,7 +7258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7210,7 +7266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7218,7 +7274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7226,7 +7282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7234,7 +7290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>119</v>
       </c>
@@ -7254,19 +7310,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7274,7 +7330,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7282,7 +7338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7290,7 +7346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7298,7 +7354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7306,7 +7362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7314,7 +7370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7322,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7330,7 +7386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7338,7 +7394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7346,7 +7402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7354,7 +7410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7362,7 +7418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7370,7 +7426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7378,7 +7434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7386,7 +7442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7394,7 +7450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7402,7 +7458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7410,7 +7466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-10 10:23:49
Affected files:
Too many files to list
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="903" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE27C318-CFBC-4280-9DAB-168CE9CAC96A}"/>
+  <xr:revisionPtr revIDLastSave="924" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67E4D7B-EA09-484A-9A65-0DB8C6B7DC57}"/>
   <bookViews>
-    <workbookView xWindow="-19395" yWindow="4050" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="16200" yWindow="7320" windowWidth="21588" windowHeight="14388" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="403">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1247,6 +1247,33 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/4127911752/?trackingId=P1ghrR8o3oaZGoDaeLKXiA%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D8d299bb8...ead4a064%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=1JijpxNTFgpHE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m75kqt9z~7h-null-null&amp;eid=1j75g-m75kqt9z-7h&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUzNDMxNmUxYjY4OWM4ZDg0NzlhYTQ4NzZmNzdjMTAwNmU0NzViNTZmNDhjODZiM2I5MTNkYWQxMWQxYjUyMmQ3NzUwNTA4ZGMzZWE4Y2UzNTZjYWFlNjEsMSwx</t>
+  </si>
+  <si>
+    <t>3/5/2025`</t>
+  </si>
+  <si>
+    <t>Interview w/ management</t>
+  </si>
+  <si>
+    <t>First interview</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>Senior Engineer Market Evaluation</t>
+  </si>
+  <si>
+    <t>application, MISO market efficiency evaluator</t>
+  </si>
+  <si>
+    <t>https://recruiting.ultipro.com/MID1029MISO/JobBoard/362b6b1d-f1c3-46f5-9554-4aa90e2bda64/OpportunityDetail?opportunityId=ae933cb8-99a0-42af-ae01-b41431abde3a</t>
+  </si>
+  <si>
+    <t>same url as before</t>
+  </si>
+  <si>
+    <t>the energy job, same url as before</t>
   </si>
 </sst>
 </file>
@@ -4591,10 +4618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
@@ -6432,6 +6459,9 @@
       <c r="D102" t="s">
         <v>374</v>
       </c>
+      <c r="E102" t="s">
+        <v>51</v>
+      </c>
       <c r="F102" t="s">
         <v>376</v>
       </c>
@@ -6542,6 +6572,60 @@
       </c>
       <c r="F108" s="5" t="s">
         <v>393</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>394</v>
+      </c>
+      <c r="B109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C109" t="s">
+        <v>373</v>
+      </c>
+      <c r="D109" t="s">
+        <v>395</v>
+      </c>
+      <c r="E109" t="s">
+        <v>51</v>
+      </c>
+      <c r="F109" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="3">
+        <v>45723</v>
+      </c>
+      <c r="B110" t="s">
+        <v>287</v>
+      </c>
+      <c r="C110" t="s">
+        <v>93</v>
+      </c>
+      <c r="D110" t="s">
+        <v>396</v>
+      </c>
+      <c r="F110" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="3">
+        <v>45724</v>
+      </c>
+      <c r="B111" t="s">
+        <v>397</v>
+      </c>
+      <c r="C111" t="s">
+        <v>398</v>
+      </c>
+      <c r="D111" t="s">
+        <v>399</v>
+      </c>
+      <c r="F111" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-13 00:45:46
Affected files:
.gitignore
obsidian/Obsidian Share Vault/.obsidian/community-plugins.json
obsidian/Obsidian Share Vault/.obsidian/workspace.json
obsidian/Obsidian Share Vault/Dailies/2023-10-20.md
obsidian/Obsidian Share Vault/Dailies/2025-03-12.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Ambler23dataModeling101.md
obsidian/Obsidian Share Vault/lit/lit_notes/Grose24youngWimynWillTalkSexistm.md
obsidian/Obsidian Share Vault/lit/lit_notes/MongoDB24noSQLVsSQLdatabases.md
obsidian/Obsidian Share Vault/tmp new.md
obsidian/Obsidian Share Vault/tmp3.md
refwrangle/zmknote/__pycache__/zotero_to_obsidian_note.cpython-313.pyc
refwrangle/zmknote/tmp.ipynb
refwrangle/zmknote/tmp/zotero_to_obsidian_output.md
refwrangle/zmknote/zotero_note_to_markdown_test_SAVE_2.py
zotero_to_obsidian_output.md
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="924" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67E4D7B-EA09-484A-9A65-0DB8C6B7DC57}"/>
+  <xr:revisionPtr revIDLastSave="925" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0A002A-FF8A-4627-972A-C05EF248605E}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="7320" windowWidth="21588" windowHeight="14388" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="403">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4620,30 +4620,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="29.19921875" customWidth="1"/>
+    <col min="4" max="4" width="46.796875" customWidth="1"/>
+    <col min="5" max="5" width="8.53125" customWidth="1"/>
+    <col min="6" max="6" width="28.19921875" customWidth="1"/>
+    <col min="7" max="7" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>45523</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>45525</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>45528</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>45530</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>45531</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>45534</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4779,7 +4779,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>45539</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>45539</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>45539</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>45540</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>45541</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>45541</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>45543</v>
       </c>
@@ -4914,7 +4914,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>45547</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>45548</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>45549</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>45555</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>45555</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>45555</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
         <v>45555</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>45562</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
         <v>45563</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
         <v>45563</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
         <v>45563</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
         <v>45563</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="3">
         <v>45563</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="3">
         <v>45563</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="3">
         <v>45566</v>
       </c>
@@ -5171,11 +5171,14 @@
       <c r="D31" t="s">
         <v>121</v>
       </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
       <c r="F31" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>45569</v>
       </c>
@@ -5192,7 +5195,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="3">
         <v>45570</v>
       </c>
@@ -5209,7 +5212,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>45577</v>
       </c>
@@ -5229,7 +5232,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="3">
         <v>45577</v>
       </c>
@@ -5249,7 +5252,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="3">
         <v>45577</v>
       </c>
@@ -5266,7 +5269,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="3">
         <v>45591</v>
       </c>
@@ -5286,7 +5289,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="3">
         <v>45591</v>
       </c>
@@ -5303,7 +5306,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="3">
         <v>45591</v>
       </c>
@@ -5323,7 +5326,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="3">
         <v>45595</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="3">
         <v>45598</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="3">
         <v>45598</v>
       </c>
@@ -5377,7 +5380,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="3">
         <v>45600</v>
       </c>
@@ -5394,7 +5397,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="3">
         <v>45600</v>
       </c>
@@ -5411,7 +5414,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="3">
         <v>45605</v>
       </c>
@@ -5431,7 +5434,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -5451,7 +5454,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="3">
         <v>45612</v>
       </c>
@@ -5468,7 +5471,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="3">
         <v>45612</v>
       </c>
@@ -5488,7 +5491,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="3">
         <v>45612</v>
       </c>
@@ -5505,7 +5508,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="13">
         <v>45616</v>
       </c>
@@ -5522,7 +5525,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="3">
         <v>45619</v>
       </c>
@@ -5539,7 +5542,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="3">
         <v>45619</v>
       </c>
@@ -5556,7 +5559,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="3">
         <v>45619</v>
       </c>
@@ -5576,7 +5579,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="3">
         <v>45626</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="3">
         <v>45626</v>
       </c>
@@ -5616,7 +5619,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="3">
         <v>45626</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="3">
         <v>45633</v>
       </c>
@@ -5653,7 +5656,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="3">
         <v>45633</v>
       </c>
@@ -5670,7 +5673,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>45633</v>
       </c>
@@ -5687,7 +5690,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>45635</v>
       </c>
@@ -5704,7 +5707,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>45640</v>
       </c>
@@ -5724,7 +5727,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="3">
         <v>45640</v>
       </c>
@@ -5741,7 +5744,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="3">
         <v>45640</v>
       </c>
@@ -5758,7 +5761,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="3">
         <v>45641</v>
       </c>
@@ -5775,7 +5778,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="3">
         <v>45647</v>
       </c>
@@ -5795,7 +5798,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="3">
         <v>45647</v>
       </c>
@@ -5812,7 +5815,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="3">
         <v>45647</v>
       </c>
@@ -5829,7 +5832,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="3">
         <v>45647</v>
       </c>
@@ -5849,7 +5852,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="3">
         <v>45651</v>
       </c>
@@ -5866,7 +5869,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="3">
         <v>45651</v>
       </c>
@@ -5886,7 +5889,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="3">
         <v>45654</v>
       </c>
@@ -5903,7 +5906,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="3">
         <v>45654</v>
       </c>
@@ -5920,7 +5923,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="3">
         <v>45654</v>
       </c>
@@ -5937,7 +5940,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="3">
         <v>45661</v>
       </c>
@@ -5957,7 +5960,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="3">
         <v>45661</v>
       </c>
@@ -5974,7 +5977,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="3">
         <v>45661</v>
       </c>
@@ -5994,7 +5997,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="3">
         <v>45667</v>
       </c>
@@ -6014,7 +6017,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="3">
         <v>45668</v>
       </c>
@@ -6034,7 +6037,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="3">
         <v>45668</v>
       </c>
@@ -6054,7 +6057,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="3">
         <v>45668</v>
       </c>
@@ -6071,7 +6074,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="3">
         <v>45668</v>
       </c>
@@ -6088,7 +6091,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="3">
         <v>45674</v>
       </c>
@@ -6108,7 +6111,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="3">
         <v>45674</v>
       </c>
@@ -6125,7 +6128,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="3">
         <v>45675</v>
       </c>
@@ -6142,7 +6145,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="3">
         <v>45682</v>
       </c>
@@ -6159,7 +6162,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="3">
         <v>45682</v>
       </c>
@@ -6176,7 +6179,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="3">
         <v>45682</v>
       </c>
@@ -6196,7 +6199,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="3">
         <v>45682</v>
       </c>
@@ -6213,7 +6216,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="3">
         <v>45316</v>
       </c>
@@ -6230,7 +6233,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="3">
         <v>45688</v>
       </c>
@@ -6247,7 +6250,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="3">
         <v>45689</v>
       </c>
@@ -6267,7 +6270,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="3">
         <v>45689</v>
       </c>
@@ -6287,7 +6290,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="3">
         <v>45689</v>
       </c>
@@ -6310,7 +6313,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="3">
         <v>45696</v>
       </c>
@@ -6327,7 +6330,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="3">
         <v>45696</v>
       </c>
@@ -6344,7 +6347,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="3">
         <v>45696</v>
       </c>
@@ -6361,7 +6364,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="3">
         <v>45696</v>
       </c>
@@ -6378,7 +6381,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="3">
         <v>45703</v>
       </c>
@@ -6395,7 +6398,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="3">
         <v>45703</v>
       </c>
@@ -6412,7 +6415,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="3">
         <v>45703</v>
       </c>
@@ -6429,7 +6432,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="3">
         <v>45703</v>
       </c>
@@ -6446,7 +6449,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="3">
         <v>45708</v>
       </c>
@@ -6469,7 +6472,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" s="3">
         <v>45710</v>
       </c>
@@ -6489,7 +6492,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>377</v>
       </c>
@@ -6506,7 +6509,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" s="3">
         <v>45717</v>
       </c>
@@ -6523,7 +6526,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="3">
         <v>45717</v>
       </c>
@@ -6540,7 +6543,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" s="3">
         <v>45717</v>
       </c>
@@ -6557,7 +6560,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="3">
         <v>45717</v>
       </c>
@@ -6574,7 +6577,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>394</v>
       </c>
@@ -6594,7 +6597,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" s="3">
         <v>45723</v>
       </c>
@@ -6611,7 +6614,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="3">
         <v>45724</v>
       </c>
@@ -6651,22 +6654,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -6686,7 +6689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -6700,7 +6703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -6717,7 +6720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -6737,7 +6740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -6754,7 +6757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -6771,7 +6774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -6785,7 +6788,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -6802,7 +6805,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45539</v>
       </c>
@@ -6822,7 +6825,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45539</v>
       </c>
@@ -6839,7 +6842,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45539</v>
       </c>
@@ -6856,7 +6859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45540</v>
       </c>
@@ -6876,7 +6879,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45541</v>
       </c>
@@ -6893,7 +6896,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45541</v>
       </c>
@@ -6913,7 +6916,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45543</v>
       </c>
@@ -6933,7 +6936,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45547</v>
       </c>
@@ -6950,7 +6953,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C22" s="3">
         <v>45548</v>
       </c>
@@ -6967,7 +6970,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C23" s="3">
         <v>45549</v>
       </c>
@@ -6984,7 +6987,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C24" s="3">
         <v>45555</v>
       </c>
@@ -7004,7 +7007,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C25" s="3">
         <v>45555</v>
       </c>
@@ -7021,7 +7024,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C26" s="3">
         <v>45555</v>
       </c>
@@ -7038,7 +7041,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C27" s="3">
         <v>45555</v>
       </c>
@@ -7055,7 +7058,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>82</v>
       </c>
@@ -7072,7 +7075,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C29" s="3">
         <v>45563</v>
       </c>
@@ -7089,7 +7092,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C30" s="3">
         <v>45563</v>
       </c>
@@ -7106,7 +7109,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C31" s="3">
         <v>45563</v>
       </c>
@@ -7123,7 +7126,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C32" s="3">
         <v>45563</v>
       </c>
@@ -7140,7 +7143,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C33" s="3">
         <v>45563</v>
       </c>
@@ -7157,7 +7160,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C34" s="3">
         <v>45563</v>
       </c>
@@ -7185,23 +7188,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C4" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C5" cm="1">
         <f t="array" ref="C5">IF(SUM(ISERROR(Sheet2!$C$7:$H$34)*1)&gt;0,NA(),COUNTA(_xlfn.UNIQUE(Sheet2!$C$7:$C$34)))</f>
         <v>17</v>
@@ -7218,19 +7221,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7238,7 +7241,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7246,7 +7249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7254,7 +7257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7262,7 +7265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7270,7 +7273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7278,7 +7281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7286,7 +7289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7294,7 +7297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7302,7 +7305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7310,7 +7313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7318,7 +7321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7326,7 +7329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7334,7 +7337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7342,7 +7345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7350,7 +7353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7358,7 +7361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7366,7 +7369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7374,7 +7377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>119</v>
       </c>
@@ -7394,19 +7397,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7414,7 +7417,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7422,7 +7425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7430,7 +7433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7438,7 +7441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7446,7 +7449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7454,7 +7457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7462,7 +7465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7470,7 +7473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7478,7 +7481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7486,7 +7489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7494,7 +7497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7502,7 +7505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7510,7 +7513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7518,7 +7521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7526,7 +7529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7534,7 +7537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7542,7 +7545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7550,7 +7553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-16 11:20:46
Affected files:
.gitignore
obsidian/Obsidian Share Vault/.obsidian/workspace.json
obsidian/Obsidian Share Vault/Dailies/2024-04-11.md
obsidian/Obsidian Share Vault/Politics/Political Causality/US Elections 2024.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Atrioc25teslaBacklashBiblical.md
obsidian/Obsidian Share Vault/lit/lit_notes/Economist25tenIndicatorsUSecon.md
obsidian/Obsidian Share Vault/lit/lit_notes/Razzaque25trumperBelievePsych.md
obsidian/Obsidian Share Vault/lit/lit_notes/attachments/image.png
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="925" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0A002A-FF8A-4627-972A-C05EF248605E}"/>
+  <xr:revisionPtr revIDLastSave="972" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F4D0FF-BCFA-4321-A70F-EBF463127437}"/>
   <bookViews>
     <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="424">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1274,6 +1274,69 @@
   </si>
   <si>
     <t>the energy job, same url as before</t>
+  </si>
+  <si>
+    <t>Principal Data Scientist, Forecasting, ASIN Forecasting</t>
+  </si>
+  <si>
+    <t>demand forecasting</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4137885098/?trackingId=e299vDboTfLyewOezp%2F49Q%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D39f6ef31...df0aa05c%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=0b_0l8pijg0XI1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m89l2nn0~g1-null-null&amp;eid=1j75g-m89l2nn0-g1&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWU4NDYxZWUyYjA4OWNkZDU0NDliYTQ4NzZmNzdjMTAwNmU0NzViNTY5NThlOWZiN2EzNjhmYWYzOTFhN2JiZmU2OTkzNjc3ZjdlYjYzNWJjY2FhYTY1YTAsMSwx</t>
+  </si>
+  <si>
+    <t>Sr. Data Scientist, Perceptor (Kumo Analytics), AWS Support</t>
+  </si>
+  <si>
+    <t>business stuff?  They mention forecasting</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4184889780/?trackingId=8RyyZELEcPLpz3qE5hd%2BFA%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D39f6ef31...df0aa05c%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=0b_0l8pijg0XI1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m89l2nn0~g1-null-null&amp;eid=1j75g-m89l2nn0-g1&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWU4NDYxZWUyYjA4OWNkZDU0NDliYTQ4NzZmNzdjMTAwNmU0NzViNTY5NThlOWZiN2EzNjhmYWYzOTFhN2JiZmU2OTkzNjc3ZjdlYjYzNWJjY2FhYTY1YTAsMSwx</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist, Last Mile Science</t>
+  </si>
+  <si>
+    <t>logistics?  Mention forecasting</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4184242488/?trackingId=EQII1MqLI2PsUdCmISGePw%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D002c1553...c1ec6cde%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=0YR_8CJIUw_HE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m88528ge~mh-null-null&amp;eid=1j75g-m88528ge-mh&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWViNGYxZmVmYjU4ZmNiZDM0OTllYTQ4NzZmNzdjMTAwNmU0NzViNTY4MWFhYWViNDgzMTNiOGIxMzY1NWE1NTY3ZDA1NzdkNmM0NjcyMTI5OWIyYmM3NzcsMSwx</t>
+  </si>
+  <si>
+    <t>Data Scientist, Topline Forecasting</t>
+  </si>
+  <si>
+    <t>Biz forecasting</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4007093976/?trackingId=GXAgJQcAHrymvJVwxCcwfQ%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D96b02801...3f23e2c7%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=3GhlV4E8MsYXE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m85cbosa~6t-null-null&amp;eid=1j75g-m85cbosa-6t&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWViNDExYWVmYmQ4ZWNkZDY0NzlmYTQ4NzZmNzdjMTAwNmU0NzViNTY5OTgyZDRhMTk5NTRmMWZmZTFlMjE1NzI2M2E1MWU0ODBmYjQ3OTI3ZTg2ODA5NjMsMSwx</t>
+  </si>
+  <si>
+    <t>Sr. Data Scientist, Devices Decision Scienc</t>
+  </si>
+  <si>
+    <t>biz stuff, mention forecasting</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4148960536/?trackingId=zHv7uEAnsa0%2FK6LDHqPWow%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D4987540d...389951e1%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=2wsph5SHHgRHE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m7y5jufr~ei-null-null&amp;eid=1j75g-m7y5jufr-ei&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWViNDUxZmUzYjY4OWNhZDU0NjkwYTQ4NzZmNzdjMTAwNmU0NzViNTZiOWY0OTNhMTkwNTRlNWZiNDVkOTEyYTY5ZGYwNWJkOWEwNzRiYjg5MGQ2OTAxNTIsMSwx</t>
+  </si>
+  <si>
+    <t>Sr. Applied Scientist, Renewable Energy Optimization</t>
+  </si>
+  <si>
+    <t>RES opt but want forecasting experience</t>
+  </si>
+  <si>
+    <t>https://www.amazon.jobs/en/jobs/2913322/sr-applied-scientist-renewable-energy-optimization?cmpid=DA_INAD200785B</t>
+  </si>
+  <si>
+    <t>Strella</t>
+  </si>
+  <si>
+    <t>produce transport decisions, I think, Seattle</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4175135972/?refId=ByteString(length%3D16%2Cbytes%3D8a8662a5...2cc15d02)&amp;trackingId=Ib7%2BrwAH6ArYZYJILpsqvg%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -4618,11 +4681,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6326,6 +6389,9 @@
       <c r="D94" t="s">
         <v>345</v>
       </c>
+      <c r="E94" t="s">
+        <v>51</v>
+      </c>
       <c r="F94" t="s">
         <v>344</v>
       </c>
@@ -6394,6 +6460,9 @@
       <c r="D98" t="s">
         <v>357</v>
       </c>
+      <c r="E98" t="s">
+        <v>51</v>
+      </c>
       <c r="F98" t="s">
         <v>358</v>
       </c>
@@ -6428,6 +6497,9 @@
       <c r="D100" t="s">
         <v>364</v>
       </c>
+      <c r="E100" t="s">
+        <v>51</v>
+      </c>
       <c r="F100" t="s">
         <v>365</v>
       </c>
@@ -6629,6 +6701,125 @@
       </c>
       <c r="F111" t="s">
         <v>400</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A112" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B112" t="s">
+        <v>19</v>
+      </c>
+      <c r="C112" t="s">
+        <v>403</v>
+      </c>
+      <c r="D112" t="s">
+        <v>404</v>
+      </c>
+      <c r="F112" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A113" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B113" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113" t="s">
+        <v>406</v>
+      </c>
+      <c r="D113" t="s">
+        <v>407</v>
+      </c>
+      <c r="F113" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A114" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B114" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114" t="s">
+        <v>409</v>
+      </c>
+      <c r="D114" t="s">
+        <v>410</v>
+      </c>
+      <c r="F114" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A115" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B115" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" t="s">
+        <v>412</v>
+      </c>
+      <c r="D115" t="s">
+        <v>413</v>
+      </c>
+      <c r="F115" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A116" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B116" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" t="s">
+        <v>415</v>
+      </c>
+      <c r="D116" t="s">
+        <v>416</v>
+      </c>
+      <c r="F116" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A117" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B117" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117" t="s">
+        <v>418</v>
+      </c>
+      <c r="D117" t="s">
+        <v>419</v>
+      </c>
+      <c r="F117" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A118" s="3">
+        <v>45731</v>
+      </c>
+      <c r="B118" t="s">
+        <v>421</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>422</v>
+      </c>
+      <c r="F118" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-27 14:25:35
Affected files:
obsidian/Obsidian Share Vault/.obsidian/community-plugins.json
obsidian/Obsidian Share Vault/.smart-env/multi/Obsidian_Obsidian_and_GIT_Repo_md.ajson
obsidian/Obsidian Share Vault/.smart-env/multi/lit_refwrangle_Zotero_to_Obsidian_to_RAG_md.ajson
obsidian/Obsidian Share Vault/Dailies/2025-03-03.md
obsidian/Obsidian Share Vault/Dailies/2025-03-27.md
obsidian/Obsidian Share Vault/Obsidian/Obsidian Multicomputer Sync.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/refwrangle/YouTube Transcripts into Obsidian Lit Notes.md
obsidian/Obsidian Share Vault/lit/refwrangle/Zotero to Obsidian to RAG.md
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1000" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6206A3DA-8278-4038-BE4C-61C76CFE2E5C}"/>
+  <xr:revisionPtr revIDLastSave="1001" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C142938F-6948-4941-BD48-71321D8849FE}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="439">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4729,8 +4729,8 @@
   <dimension ref="A1:G123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F123" sqref="F123"/>
+      <pane ySplit="2" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6453,6 +6453,9 @@
       </c>
       <c r="D95" t="s">
         <v>346</v>
+      </c>
+      <c r="E95" t="s">
+        <v>51</v>
       </c>
       <c r="F95" t="s">
         <v>347</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-03-31 04:45:01
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1001" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C142938F-6948-4941-BD48-71321D8849FE}"/>
+  <xr:revisionPtr revIDLastSave="1008" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9F5CCFF-1FC2-4A52-8B2C-B1089FF35702}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="442">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1381,7 +1381,16 @@
     <t>Habitat Energy</t>
   </si>
   <si>
-    <t>Austin, Bradley Davidson is HH</t>
+    <t>Austin, Bradley Davidson is HH, talk withthem</t>
+  </si>
+  <si>
+    <t>Blue Rose Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine Learning Engineer </t>
+  </si>
+  <si>
+    <t>Remote, David Shor's polling company</t>
   </si>
 </sst>
 </file>
@@ -4726,11 +4735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6940,7 +6949,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="3">
-        <v>45376</v>
+        <v>45741</v>
       </c>
       <c r="B123" t="s">
         <v>437</v>
@@ -6950,6 +6959,20 @@
       </c>
       <c r="D123" t="s">
         <v>438</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" s="3">
+        <v>45746</v>
+      </c>
+      <c r="B124" t="s">
+        <v>439</v>
+      </c>
+      <c r="C124" t="s">
+        <v>440</v>
+      </c>
+      <c r="D124" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-04-10 12:27:58
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/Interview Projects/Habitat Energy 2025/Basic two sided scen clust pyomo Perplexity smc.md
obsidian/Obsidian Share Vault/Work/Between Jobs/Interview Projects/Habitat Energy 2025/My Notes - Habitat 2025.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1015" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70F374AF-12C5-41FF-88B0-C823DC27F1CA}"/>
+  <xr:revisionPtr revIDLastSave="1016" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE77B39A-4116-4C4B-9C55-26D00C3D9138}"/>
   <bookViews>
     <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="444">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4744,8 +4744,8 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6024,6 +6024,9 @@
       </c>
       <c r="D71" t="s">
         <v>255</v>
+      </c>
+      <c r="E71" t="s">
+        <v>51</v>
       </c>
       <c r="F71" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-04-17 12:03:34
Affected files:
obsidian/Obsidian Share Vault/.obsidian/hotkeys.json
obsidian/Obsidian Share Vault/Obsidian/Arrow and Tab Key Mapping.md
obsidian/Obsidian Share Vault/Work/Between Jobs/Interview Projects/Habitat Energy 2025/My Notes - Habitat 2025.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Gao20lelecMktProbFrcstStochProg.md
obsidian/Obsidian Share Vault/lit/lit_notes/Laws23priceGenElecMktBidEval.md
obsidian/Obsidian Share Vault/lit/lit_notes/Mones23stochOptConvergBid.md
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1016" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE77B39A-4116-4C4B-9C55-26D00C3D9138}"/>
+  <xr:revisionPtr revIDLastSave="1017" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5D17F83-AFF1-4684-A762-68302D81558D}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="4224" yWindow="4224" windowWidth="34560" windowHeight="18984" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="444">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4744,29 +4744,29 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+      <pane ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" customWidth="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="29.19921875" customWidth="1"/>
-    <col min="4" max="4" width="46.796875" customWidth="1"/>
-    <col min="5" max="5" width="8.53125" customWidth="1"/>
-    <col min="6" max="6" width="28.19921875" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45523</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45525</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>45528</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>45530</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>45531</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>45534</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45539</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45539</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>45539</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>45540</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>45541</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>45541</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>45543</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>45547</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>45548</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>45549</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45555</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>45555</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>45555</v>
       </c>
@@ -5142,7 +5142,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>45555</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>45562</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>45563</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>45563</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>45563</v>
       </c>
@@ -5227,7 +5227,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>45563</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45563</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>45563</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>45566</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>45569</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>45570</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>45577</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>45577</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>45577</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>45591</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>45591</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>45591</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>45595</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>45598</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>45598</v>
       </c>
@@ -5503,7 +5503,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>45600</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>45600</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>45605</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -5577,7 +5577,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45612</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>45612</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>45612</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>45616</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>45619</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>45619</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>45619</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>45626</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>45626</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>45626</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>45633</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>45633</v>
       </c>
@@ -5792,11 +5792,14 @@
       <c r="D58" t="s">
         <v>216</v>
       </c>
+      <c r="E58" t="s">
+        <v>51</v>
+      </c>
       <c r="F58" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>45633</v>
       </c>
@@ -5813,7 +5816,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>45635</v>
       </c>
@@ -5830,7 +5833,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>45640</v>
       </c>
@@ -5850,7 +5853,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>45640</v>
       </c>
@@ -5867,7 +5870,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>45640</v>
       </c>
@@ -5884,7 +5887,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>45641</v>
       </c>
@@ -5901,7 +5904,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>45647</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>45647</v>
       </c>
@@ -5938,7 +5941,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>45647</v>
       </c>
@@ -5955,7 +5958,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>45647</v>
       </c>
@@ -5975,7 +5978,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>45651</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>45651</v>
       </c>
@@ -6012,7 +6015,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>45654</v>
       </c>
@@ -6032,7 +6035,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>45654</v>
       </c>
@@ -6049,7 +6052,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>45654</v>
       </c>
@@ -6066,7 +6069,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>45661</v>
       </c>
@@ -6086,7 +6089,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>45661</v>
       </c>
@@ -6103,7 +6106,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>45661</v>
       </c>
@@ -6123,7 +6126,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>45667</v>
       </c>
@@ -6143,7 +6146,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>45668</v>
       </c>
@@ -6163,7 +6166,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>45668</v>
       </c>
@@ -6183,7 +6186,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>45668</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>45668</v>
       </c>
@@ -6217,7 +6220,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>45674</v>
       </c>
@@ -6237,7 +6240,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>45674</v>
       </c>
@@ -6254,7 +6257,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>45675</v>
       </c>
@@ -6271,7 +6274,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>45682</v>
       </c>
@@ -6288,7 +6291,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>45682</v>
       </c>
@@ -6305,7 +6308,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>45682</v>
       </c>
@@ -6325,7 +6328,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>45682</v>
       </c>
@@ -6342,7 +6345,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>45316</v>
       </c>
@@ -6359,7 +6362,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>45688</v>
       </c>
@@ -6376,7 +6379,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>45689</v>
       </c>
@@ -6396,7 +6399,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>45689</v>
       </c>
@@ -6416,7 +6419,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>45689</v>
       </c>
@@ -6439,7 +6442,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>45696</v>
       </c>
@@ -6459,7 +6462,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>45696</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>45696</v>
       </c>
@@ -6496,7 +6499,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>45696</v>
       </c>
@@ -6513,7 +6516,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>45703</v>
       </c>
@@ -6533,7 +6536,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>45703</v>
       </c>
@@ -6550,7 +6553,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>45703</v>
       </c>
@@ -6570,7 +6573,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>45703</v>
       </c>
@@ -6587,7 +6590,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>45708</v>
       </c>
@@ -6610,7 +6613,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>45710</v>
       </c>
@@ -6630,7 +6633,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>377</v>
       </c>
@@ -6647,7 +6650,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>45717</v>
       </c>
@@ -6664,7 +6667,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>45717</v>
       </c>
@@ -6681,7 +6684,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>45717</v>
       </c>
@@ -6698,7 +6701,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>45717</v>
       </c>
@@ -6715,7 +6718,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>394</v>
       </c>
@@ -6735,7 +6738,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>45723</v>
       </c>
@@ -6752,7 +6755,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>45724</v>
       </c>
@@ -6769,7 +6772,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>45731</v>
       </c>
@@ -6786,7 +6789,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>45731</v>
       </c>
@@ -6803,7 +6806,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>45731</v>
       </c>
@@ -6820,7 +6823,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>45731</v>
       </c>
@@ -6837,7 +6840,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>45731</v>
       </c>
@@ -6854,7 +6857,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>45731</v>
       </c>
@@ -6871,7 +6874,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>45731</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>45739</v>
       </c>
@@ -6908,7 +6911,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>45739</v>
       </c>
@@ -6925,7 +6928,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>45739</v>
       </c>
@@ -6942,7 +6945,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>45740</v>
       </c>
@@ -6956,7 +6959,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>45741</v>
       </c>
@@ -6970,7 +6973,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>45746</v>
       </c>
@@ -6984,7 +6987,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>45748</v>
       </c>
@@ -7021,22 +7024,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -7056,7 +7059,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7070,7 +7073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7087,7 +7090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7107,7 +7110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7124,7 +7127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7141,7 +7144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7155,7 +7158,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -7172,7 +7175,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45539</v>
       </c>
@@ -7192,7 +7195,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45539</v>
       </c>
@@ -7209,7 +7212,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45539</v>
       </c>
@@ -7226,7 +7229,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45540</v>
       </c>
@@ -7246,7 +7249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45541</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45541</v>
       </c>
@@ -7283,7 +7286,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45543</v>
       </c>
@@ -7303,7 +7306,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45547</v>
       </c>
@@ -7320,7 +7323,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>45548</v>
       </c>
@@ -7337,7 +7340,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>45549</v>
       </c>
@@ -7354,7 +7357,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>45555</v>
       </c>
@@ -7374,7 +7377,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>45555</v>
       </c>
@@ -7391,7 +7394,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>45555</v>
       </c>
@@ -7408,7 +7411,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" s="3">
         <v>45555</v>
       </c>
@@ -7425,7 +7428,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>82</v>
       </c>
@@ -7442,7 +7445,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>45563</v>
       </c>
@@ -7459,7 +7462,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>45563</v>
       </c>
@@ -7476,7 +7479,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
         <v>45563</v>
       </c>
@@ -7493,7 +7496,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>45563</v>
       </c>
@@ -7510,7 +7513,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C33" s="3">
         <v>45563</v>
       </c>
@@ -7527,7 +7530,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
         <v>45563</v>
       </c>
@@ -7555,23 +7558,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C5" cm="1">
         <f t="array" ref="C5">IF(SUM(ISERROR(Sheet2!$C$7:$H$34)*1)&gt;0,NA(),COUNTA(_xlfn.UNIQUE(Sheet2!$C$7:$C$34)))</f>
         <v>17</v>
@@ -7588,19 +7591,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7608,7 +7611,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7616,7 +7619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7624,7 +7627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7632,7 +7635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7640,7 +7643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7648,7 +7651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7656,7 +7659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7664,7 +7667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7672,7 +7675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7680,7 +7683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7688,7 +7691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7696,7 +7699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7704,7 +7707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7712,7 +7715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7720,7 +7723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7728,7 +7731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7736,7 +7739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7744,7 +7747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>119</v>
       </c>
@@ -7764,19 +7767,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -7784,7 +7787,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -7792,7 +7795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -7800,7 +7803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7808,7 +7811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7816,7 +7819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7824,7 +7827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7832,7 +7835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7840,7 +7843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7848,7 +7851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -7856,7 +7859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -7864,7 +7867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -7872,7 +7875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -7880,7 +7883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -7888,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -7896,7 +7899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -7904,7 +7907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -7912,7 +7915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -7920,7 +7923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-04-30 04:44:24
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1027" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{009B5C6C-89C1-4F15-89E1-5E81F37DC0AD}"/>
+  <xr:revisionPtr revIDLastSave="1042" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C5E95AD-E54E-4B9D-B4FB-515EF2D955F9}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="454">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1406,6 +1406,27 @@
   </si>
   <si>
     <t>Seattle, do some energy, but not this job</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>Data Scientist I</t>
+  </si>
+  <si>
+    <t>https://www.indeed.com/viewjob?jk=60c0b6dfe3e94510&amp;q=data+scientist+energy&amp;l=Seattle%2C+WA&amp;tk=1iq2n9d8vgh70800&amp;from=ja&amp;alid=57572b3de4b0d72084d4c871&amp;xpse=SoCH67I3yC8SjnQVgR0LbzkdCdPP&amp;xfps=35b8393f-880b-4312-b6d7-94624e0086ab&amp;rgtk=1iq2n9d8vgh70800&amp;xkcb=SoDz67M3yCmqAB0_SB0IbzkdCdPP</t>
+  </si>
+  <si>
+    <t>Gridmatic</t>
+  </si>
+  <si>
+    <t>Cupertino, CA: bummer</t>
+  </si>
+  <si>
+    <t>Data Scientist (optimization)</t>
+  </si>
+  <si>
+    <t>Austin, TX.  I sent in my takehome project</t>
   </si>
 </sst>
 </file>
@@ -3912,6 +3933,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4749,11 +4774,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E125" sqref="E125"/>
+      <pane ySplit="2" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7036,6 +7061,51 @@
       </c>
       <c r="F126" s="16" t="s">
         <v>445</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A127" s="3">
+        <v>45777</v>
+      </c>
+      <c r="B127" t="s">
+        <v>447</v>
+      </c>
+      <c r="C127" t="s">
+        <v>448</v>
+      </c>
+      <c r="D127" t="s">
+        <v>257</v>
+      </c>
+      <c r="F127" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="3">
+        <v>45772</v>
+      </c>
+      <c r="B128" t="s">
+        <v>450</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A129" s="3">
+        <v>45774</v>
+      </c>
+      <c r="B129" t="s">
+        <v>437</v>
+      </c>
+      <c r="C129" t="s">
+        <v>452</v>
+      </c>
+      <c r="D129" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-05-09 16:47:13
Affected files:
obsidian/Obsidian Share Vault/Politics/Political Causality/US Elections 2024.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1074" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7ED8479-E6F3-4CC3-A6ED-9A73A869EDB0}"/>
+  <xr:revisionPtr revIDLastSave="1075" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{389C40E3-C0F1-4CB4-8A61-44EBF67060F8}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="472">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4273,7 +4273,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A522DF62-6C4F-4B90-B466-4C5BE7B7644D}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A522DF62-6C4F-4B90-B466-4C5BE7B7644D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="C4:D22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="ascending">
@@ -4393,7 +4393,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA556668-D747-4940-9E59-1207332A0F6C}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EA556668-D747-4940-9E59-1207332A0F6C}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="C4:D22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" sortType="ascending">
@@ -4831,9 +4831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6790,6 +6790,9 @@
       </c>
       <c r="D107" t="s">
         <v>388</v>
+      </c>
+      <c r="E107" t="s">
+        <v>51</v>
       </c>
       <c r="F107" t="s">
         <v>389</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-05-14 17:17:24
Affected files:
obsidian/Obsidian Share Vault/Dailies/2024-03-09.md
obsidian/Obsidian Share Vault/Politics/Political Causality/US Elections 2024.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Tapper25HowJoeBiden.md
obsidian/Obsidian Share Vault/lit/lit_notes/Tapper25bidenHandedTrumpPres.html.md
obsidian/Obsidian Share Vault/lit/lit_notes/Tapper25bidenHandedTrumpPres.md
obsidian/Obsidian Share Vault/lit/lit_notes/how-joe-biden-handed-the-presidency-to-donald-trump.html.md
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1075" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{389C40E3-C0F1-4CB4-8A61-44EBF67060F8}"/>
+  <xr:revisionPtr revIDLastSave="1079" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{168F3D7A-C554-4D99-B28F-03AE120F8553}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="472">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1366,9 +1366,6 @@
     <t>PacificCorps</t>
   </si>
   <si>
-    <t>I've applied for this beore, I think…</t>
-  </si>
-  <si>
     <t>https://careers.pacificorp.com/job/PORTLAND-T&amp;D-Data-Scientist-I%2C-II-Portland%2C-OR-113373-OR-97232/1274308000/?from=email&amp;refid=24007081300&amp;source=2&amp;eid=75300-202525220425-30424573000&amp;locale=en_US</t>
   </si>
   <si>
@@ -1481,6 +1478,9 @@
   </si>
   <si>
     <t>https://www.amazon.jobs/en/jobs/2970308/applied-scientist-renewable-energy-optimization?cmpid=DA_INAD200785B</t>
+  </si>
+  <si>
+    <t>I've applied for this before, I think…</t>
   </si>
 </sst>
 </file>
@@ -3988,10 +3988,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4832,8 +4828,8 @@
   <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6882,6 +6878,9 @@
       <c r="D112" t="s">
         <v>404</v>
       </c>
+      <c r="E112" t="s">
+        <v>51</v>
+      </c>
       <c r="F112" t="s">
         <v>405</v>
       </c>
@@ -7025,7 +7024,7 @@
         <v>429</v>
       </c>
       <c r="E120" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F120" t="s">
         <v>430</v>
@@ -7042,10 +7041,13 @@
         <v>431</v>
       </c>
       <c r="D121" t="s">
+        <v>471</v>
+      </c>
+      <c r="E121" t="s">
+        <v>51</v>
+      </c>
+      <c r="F121" t="s">
         <v>433</v>
-      </c>
-      <c r="F121" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.45">
@@ -7053,13 +7055,13 @@
         <v>45740</v>
       </c>
       <c r="B122" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C122" t="s">
         <v>7</v>
       </c>
       <c r="D122" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.45">
@@ -7067,13 +7069,13 @@
         <v>45741</v>
       </c>
       <c r="B123" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C123" t="s">
         <v>33</v>
       </c>
       <c r="D123" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.45">
@@ -7081,13 +7083,13 @@
         <v>45746</v>
       </c>
       <c r="B124" t="s">
+        <v>438</v>
+      </c>
+      <c r="C124" t="s">
         <v>439</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>440</v>
-      </c>
-      <c r="D124" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.45">
@@ -7095,13 +7097,13 @@
         <v>45748</v>
       </c>
       <c r="B125" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C125" t="s">
         <v>172</v>
       </c>
       <c r="D125" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -7112,13 +7114,13 @@
         <v>306</v>
       </c>
       <c r="C126" t="s">
+        <v>444</v>
+      </c>
+      <c r="D126" t="s">
         <v>445</v>
       </c>
-      <c r="D126" t="s">
-        <v>446</v>
-      </c>
       <c r="F126" s="16" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.45">
@@ -7126,16 +7128,16 @@
         <v>45777</v>
       </c>
       <c r="B127" t="s">
+        <v>446</v>
+      </c>
+      <c r="C127" t="s">
         <v>447</v>
-      </c>
-      <c r="C127" t="s">
-        <v>448</v>
       </c>
       <c r="D127" t="s">
         <v>257</v>
       </c>
       <c r="F127" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.45">
@@ -7143,13 +7145,13 @@
         <v>45772</v>
       </c>
       <c r="B128" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C128" t="s">
         <v>7</v>
       </c>
       <c r="D128" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E128" t="s">
         <v>51</v>
@@ -7160,13 +7162,13 @@
         <v>45774</v>
       </c>
       <c r="B129" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C129" t="s">
+        <v>451</v>
+      </c>
+      <c r="D129" t="s">
         <v>452</v>
-      </c>
-      <c r="D129" t="s">
-        <v>453</v>
       </c>
       <c r="E129" t="s">
         <v>51</v>
@@ -7177,16 +7179,16 @@
         <v>46878</v>
       </c>
       <c r="B130" t="s">
+        <v>454</v>
+      </c>
+      <c r="C130" t="s">
+        <v>453</v>
+      </c>
+      <c r="D130" t="s">
         <v>455</v>
       </c>
-      <c r="C130" t="s">
-        <v>454</v>
-      </c>
-      <c r="D130" t="s">
+      <c r="F130" s="5" t="s">
         <v>456</v>
-      </c>
-      <c r="F130" s="5" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.45">
@@ -7194,13 +7196,13 @@
         <v>45782</v>
       </c>
       <c r="B131" t="s">
+        <v>458</v>
+      </c>
+      <c r="C131" t="s">
+        <v>457</v>
+      </c>
+      <c r="F131" t="s">
         <v>459</v>
-      </c>
-      <c r="C131" t="s">
-        <v>458</v>
-      </c>
-      <c r="F131" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.45">
@@ -7208,16 +7210,16 @@
         <v>45782</v>
       </c>
       <c r="B132" t="s">
+        <v>461</v>
+      </c>
+      <c r="C132" t="s">
+        <v>460</v>
+      </c>
+      <c r="D132" t="s">
+        <v>463</v>
+      </c>
+      <c r="F132" t="s">
         <v>462</v>
-      </c>
-      <c r="C132" t="s">
-        <v>461</v>
-      </c>
-      <c r="D132" t="s">
-        <v>464</v>
-      </c>
-      <c r="F132" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.45">
@@ -7225,16 +7227,16 @@
         <v>45782</v>
       </c>
       <c r="B133" t="s">
+        <v>465</v>
+      </c>
+      <c r="C133" t="s">
+        <v>464</v>
+      </c>
+      <c r="D133" t="s">
         <v>466</v>
       </c>
-      <c r="C133" t="s">
-        <v>465</v>
-      </c>
-      <c r="D133" t="s">
+      <c r="F133" t="s">
         <v>467</v>
-      </c>
-      <c r="F133" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.45">
@@ -7245,13 +7247,13 @@
         <v>19</v>
       </c>
       <c r="C134" t="s">
+        <v>468</v>
+      </c>
+      <c r="D134" t="s">
         <v>469</v>
       </c>
-      <c r="D134" t="s">
+      <c r="F134" s="5" t="s">
         <v>470</v>
-      </c>
-      <c r="F134" t="s">
-        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -7267,9 +7269,10 @@
     <hyperlink ref="F108" r:id="rId9" display="https://www.linkedin.com/jobs/view/4127911752/?trackingId=P1ghrR8o3oaZGoDaeLKXiA%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D8d299bb8...ead4a064%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=1JijpxNTFgpHE1&amp;trkEmail=eml-email_job_alert_digest_01-job_card-0-jobcard_body-null-1j75g~m75kqt9z~7h-null-null&amp;eid=1j75g-m75kqt9z-7h&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwNmUzNDMxNmUxYjY4OWM4ZDg0NzlhYTQ4NzZmNzdjMTAwNmU0NzViNTZmNDhjODZiM2I5MTNkYWQxMWQxYjUyMmQ3NzUwNTA4ZGMzZWE4Y2UzNTZjYWFlNjEsMSwx" xr:uid="{96425F70-4035-4136-B80B-46A73A07E3FB}"/>
     <hyperlink ref="F126" r:id="rId10" display="https://jobs.apple.com/en-us/details/200562011/Machine-Learning-Engineer,-OS-Intelligence" xr:uid="{017F8808-46A4-4598-8116-82D13187EC3D}"/>
     <hyperlink ref="F130" r:id="rId11" xr:uid="{645ECDE8-E797-4837-992E-3B656E30BBD6}"/>
+    <hyperlink ref="F134" r:id="rId12" xr:uid="{75469FFF-1592-43D7-9958-69C7E32B0374}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="4294967295" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="4294967295" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
obsidian backup auto: 2025-05-18 09:50:35
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1079" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{168F3D7A-C554-4D99-B28F-03AE120F8553}"/>
+  <xr:revisionPtr revIDLastSave="1080" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1B186B-0BE6-4331-B9B9-058AE22508E1}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="472">
   <si>
     <t>Employment actions</t>
   </si>
@@ -3988,6 +3988,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4827,9 +4831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7234,6 +7238,9 @@
       </c>
       <c r="D133" t="s">
         <v>466</v>
+      </c>
+      <c r="E133" t="s">
+        <v>51</v>
       </c>
       <c r="F133" t="s">
         <v>467</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-06-04 17:22:16
Affected files:
obsidian/Obsidian Share Vault/.obsidian/community-plugins.json
obsidian/Obsidian Share Vault/Dailies/2024-03-23.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bbd96b3698748f8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1080" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F1B186B-0BE6-4331-B9B9-058AE22508E1}"/>
+  <xr:revisionPtr revIDLastSave="1081" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B5B1BC2-283E-42F8-8B00-B271177CA753}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="472">
   <si>
     <t>Employment actions</t>
   </si>
@@ -3988,10 +3988,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4831,9 +4827,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D133" sqref="D133"/>
+      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7204,6 +7200,9 @@
       </c>
       <c r="C131" t="s">
         <v>457</v>
+      </c>
+      <c r="E131" t="s">
+        <v>51</v>
       </c>
       <c r="F131" t="s">
         <v>459</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-06-09 17:58:05
Affected files:
obsidian/Obsidian Share Vault/.obsidian/community-plugins.json
obsidian/Obsidian Share Vault/Dailies/2024-03-23.md
obsidian/Obsidian Share Vault/Dailies/2025-06-06.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1081" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B5B1BC2-283E-42F8-8B00-B271177CA753}"/>
+  <xr:revisionPtr revIDLastSave="1083" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A84563D1-59EB-4946-AE37-413B66FF5552}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="472">
   <si>
     <t>Employment actions</t>
   </si>
@@ -3988,6 +3988,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4829,7 +4833,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
+      <selection pane="bottomLeft" activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7105,6 +7109,9 @@
       <c r="D125" t="s">
         <v>442</v>
       </c>
+      <c r="E125" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A126" s="3">
@@ -7257,6 +7264,9 @@
       </c>
       <c r="D134" t="s">
         <v>469</v>
+      </c>
+      <c r="E134" t="s">
+        <v>51</v>
       </c>
       <c r="F134" s="5" t="s">
         <v>470</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-06-10 23:09:12
Affected files:
obsidian/Obsidian Share Vault/.obsidian/backlink.json
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1083" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A84563D1-59EB-4946-AE37-413B66FF5552}"/>
+  <xr:revisionPtr revIDLastSave="1114" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95BB678A-576E-4282-86A9-A2F04C542020}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="14483" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="488">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1481,6 +1481,54 @@
   </si>
   <si>
     <t>I've applied for this before, I think…</t>
+  </si>
+  <si>
+    <t>TriCom Tech. Srvcs</t>
+  </si>
+  <si>
+    <t>Mpls, some kinda DS, want pyspark, etc. too</t>
+  </si>
+  <si>
+    <t>https://tricomts.com/thanks?submissionGuid=b7e9bcc5-ecac-4bef-9e1c-185d1287974d</t>
+  </si>
+  <si>
+    <t>Jacobs</t>
+  </si>
+  <si>
+    <t>Seattle, want 3 yrs sql and urban planning</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4240985029/?trackingId=OFLdSA2TRi2%2Fs9YyFbSz9Q%3D%3D&amp;refId=dvy6NrZQQQCjBMLe7xVjTw%3D%3D&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=12PkMqoq3USrM1&amp;trkEmail=eml-jobs_jymbii_digest-job_card-0-jobcard_body-null-1j75g~mbl0mm8z~1l-null-null&amp;eid=1j75g-mbl0mm8z-1l&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWUzNDQxY2UwYjQ4N2M4ZDc0NDkxYTQ4NzZmNzdjMTAwNmU0NzViNTZmYWI2ODI5MGEzNDNkNWZlMGQ4Y2JjOTE2ZTg2M2NjNDIxNTRlMWI2YTdjOWI0Y2IsMSwx</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist (ID:46984</t>
+  </si>
+  <si>
+    <t>Versique</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4242253047/?refId=ByteString(length%3D16%2Cbytes%3Dfabcb0fd...ab05cc36)&amp;trackingId=SXyg3cJshTb0HVK2O8sqfQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Residio</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4226498792/?trackingId=Ja9da%2FjH%2B28cifexcW8hSg%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3Dfabcb0fd...ab05cc36%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=1XrX5Uhf-9QrM1&amp;trkEmail=eml-email_job_alert_digest_01-primary_job_list-0-jobcard_body-null-1j75g~mbivgu85~qt-null-null&amp;eid=1j75g-mbivgu85-qt&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWUzNDYxN2UwYjE4YmNjZDU0MDk5YTQ4NzZmNzdjMTAwNmU0NzViNTY4YmFlZDFiNjgxNzJjNmQwMjBkM2E0YTQ3ZDEzMjMwMGNhZjUwYzlmNDZlOTA1ZWMsMSwx</t>
+  </si>
+  <si>
+    <t>Bellevue, super low pay: $110k</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4240287783/?refId=ByteString(length%3D16%2Cbytes%3D8f2f56d1...a60e75b6)&amp;trackingId=BYuILGb4CJcf1VeQWdf0sw%3D%3D</t>
+  </si>
+  <si>
+    <t>Responsible AI Data Scientist - AI Red Teamer</t>
+  </si>
+  <si>
+    <t>Salesforce</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/4243029077/?trackingId=qdWducvyXbIrk%2FDsk13u4g%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D8f2f56d1...a60e75b6%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=3VpEaHyaHgNrM1&amp;trkEmail=eml-email_job_alert_digest_01-primary_job_list-0-jobcard_body-null-1j75g~mbfwat6u~q1-null-null&amp;eid=1j75g-mbfwat6u-q1&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWUyNGYxZmUwYjA4OWNjZDY0MjlmYTQ4NzZmNzdjMTAwNmU0NzViNTZhMGE5YmRiNjlkNGJmOWU2NDNjY2QwM2FjMjY5M2MwYjIwMmFlMTk1M2Y4M2M5NWIsMSwx</t>
   </si>
 </sst>
 </file>
@@ -4829,11 +4877,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F124" sqref="F124"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7270,6 +7318,102 @@
       </c>
       <c r="F134" s="5" t="s">
         <v>470</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A135" s="3">
+        <v>45818</v>
+      </c>
+      <c r="B135" t="s">
+        <v>472</v>
+      </c>
+      <c r="C135" t="s">
+        <v>128</v>
+      </c>
+      <c r="D135" t="s">
+        <v>473</v>
+      </c>
+      <c r="F135" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A136" s="3">
+        <v>45818</v>
+      </c>
+      <c r="B136" t="s">
+        <v>475</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" t="s">
+        <v>476</v>
+      </c>
+      <c r="F136" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A137" s="3">
+        <v>45818</v>
+      </c>
+      <c r="B137" t="s">
+        <v>479</v>
+      </c>
+      <c r="C137" t="s">
+        <v>478</v>
+      </c>
+      <c r="D137" t="s">
+        <v>466</v>
+      </c>
+      <c r="F137" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A138" s="3">
+        <v>45818</v>
+      </c>
+      <c r="B138" t="s">
+        <v>481</v>
+      </c>
+      <c r="C138" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" t="s">
+        <v>466</v>
+      </c>
+      <c r="F138" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B139" t="s">
+        <v>336</v>
+      </c>
+      <c r="C139" t="s">
+        <v>61</v>
+      </c>
+      <c r="D139" t="s">
+        <v>483</v>
+      </c>
+      <c r="F139" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B140" t="s">
+        <v>486</v>
+      </c>
+      <c r="C140" t="s">
+        <v>485</v>
+      </c>
+      <c r="D140" t="s">
+        <v>257</v>
+      </c>
+      <c r="F140" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-06-11 14:51:42
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1114" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95BB678A-576E-4282-86A9-A2F04C542020}"/>
+  <xr:revisionPtr revIDLastSave="1115" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10EC877D-FBBA-4958-9FA3-34F7E32C6D43}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="14483" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="2062" yWindow="3877" windowWidth="16201" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4881,7 +4881,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C141" sqref="C141"/>
+      <selection pane="bottomLeft" activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7367,7 +7367,7 @@
       <c r="D137" t="s">
         <v>466</v>
       </c>
-      <c r="F137" t="s">
+      <c r="F137" s="5" t="s">
         <v>480</v>
       </c>
     </row>
@@ -7430,9 +7430,10 @@
     <hyperlink ref="F126" r:id="rId10" display="https://jobs.apple.com/en-us/details/200562011/Machine-Learning-Engineer,-OS-Intelligence" xr:uid="{017F8808-46A4-4598-8116-82D13187EC3D}"/>
     <hyperlink ref="F130" r:id="rId11" xr:uid="{645ECDE8-E797-4837-992E-3B656E30BBD6}"/>
     <hyperlink ref="F134" r:id="rId12" xr:uid="{75469FFF-1592-43D7-9958-69C7E32B0374}"/>
+    <hyperlink ref="F137" r:id="rId13" xr:uid="{CD5D3CDF-8C02-4D1F-82E0-7A676FA2C654}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="4294967295" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="4294967295" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
obsidian backup auto: 2025-06-13 17:04:30
Affected files:
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1115" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10EC877D-FBBA-4958-9FA3-34F7E32C6D43}"/>
+  <xr:revisionPtr revIDLastSave="1117" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E17F1F-37C4-4371-99E8-272239B766B2}"/>
   <bookViews>
-    <workbookView xWindow="2062" yWindow="3877" windowWidth="16201" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="-83" yWindow="2887" windowWidth="14483" windowHeight="10433" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4036,10 +4036,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4879,9 +4875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F137" sqref="F137"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7389,6 +7385,9 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A139" s="3">
+        <v>45818</v>
+      </c>
       <c r="B139" t="s">
         <v>336</v>
       </c>
@@ -7403,6 +7402,9 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A140" s="3">
+        <v>45818</v>
+      </c>
       <c r="B140" t="s">
         <v>486</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-06-18 00:55:26
Affected files:
obsidian/Obsidian Share Vault/Politics/Political Causality/US Elections 2024.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Brody25techAccountBigBeautBill.md
obsidian/Obsidian Share Vault/lit/lit_notes/Bump25protestsNotHelpTrump.md
obsidian/Obsidian Share Vault/lit/lit_notes/Chenoweth25protest35rule.md
obsidian/Obsidian Share Vault/lit/lit_notes/Hochschild25demsMissTrumpAppeal.md
obsidian/Obsidian Share Vault/lit/lit_notes/Klein25leftLostTrans.md
obsidian/Obsidian Share Vault/lit/lit_notes/Morris25dataDrivenTrumpCvr.md
obsidian/Obsidian Share Vault/lit/lit_notes/Morris25noKingsDay.md
obsidian/Obsidian Share Vault/lit/lit_notes/Morris25strengthNumsNewsLtr.md
obsidian/Obsidian Share Vault/lit/lit_notes/attachments/image-20.png
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1117" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E17F1F-37C4-4371-99E8-272239B766B2}"/>
+  <xr:revisionPtr revIDLastSave="1119" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A86CD1ED-FFEB-4CBE-9791-C8DAE83363F5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-83" yWindow="2887" windowWidth="14483" windowHeight="10433" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="2887" windowWidth="14483" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="489">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1529,6 +1529,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/4243029077/?trackingId=qdWducvyXbIrk%2FDsk13u4g%3D%3D&amp;refId=ByteString%28length%3D16%2Cbytes%3D8f2f56d1...a60e75b6%29&amp;midToken=AQFpnZsm4rTQjw&amp;midSig=3VpEaHyaHgNrM1&amp;trkEmail=eml-email_job_alert_digest_01-primary_job_list-0-jobcard_body-null-1j75g~mbfwat6u~q1-null-null&amp;eid=1j75g-mbfwat6u-q1&amp;otpToken=MTAwMDE5ZTUxMTJhYzFjZWI1MjkwMWUyNGYxZmUwYjA4OWNjZDY0MjlmYTQ4NzZmNzdjMTAwNmU0NzViNTZhMGE5YmRiNjlkNGJmOWU2NDNjY2QwM2FjMjY5M2MwYjIwMmFlMTk1M2Y4M2M5NWIsMSwx</t>
+  </si>
+  <si>
+    <t>Eden Prairie, MN, Hormel</t>
   </si>
 </sst>
 </file>
@@ -4036,6 +4039,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Scott Otterson" refreshedDate="45564.50100462963" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="28" xr:uid="{544BC45C-7C13-42C1-BB27-C722E465F0AB}">
   <cacheSource type="worksheet">
@@ -4877,7 +4884,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B143" sqref="B143"/>
+      <selection pane="bottomLeft" activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7346,6 +7353,9 @@
       <c r="D136" t="s">
         <v>476</v>
       </c>
+      <c r="E136" t="s">
+        <v>51</v>
+      </c>
       <c r="F136" t="s">
         <v>477</v>
       </c>
@@ -7361,7 +7371,7 @@
         <v>478</v>
       </c>
       <c r="D137" t="s">
-        <v>466</v>
+        <v>488</v>
       </c>
       <c r="F137" s="5" t="s">
         <v>480</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-07-11 18:14:55
Affected files:
obsidian/Obsidian Share Vault/Health/Exercise/Running.md
obsidian/Obsidian Share Vault/Software Dev/Tools for Software Dev/Gemini CLI.md
obsidian/Obsidian Share Vault/Software Dev/Tools for Software Dev/Source Code Control/Git Source Code Control.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Li19cmplxTrainRunNeuroEcon.md
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1170" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F4A9B04-6A67-4123-88A4-C4113E30001C}"/>
+  <xr:revisionPtr revIDLastSave="1171" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D4E657-94F6-47EB-9E86-9CC6418DEF29}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14595" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="514">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4959,7 +4959,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
+      <selection pane="bottomLeft" activeCell="F146" sqref="F146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7600,6 +7600,9 @@
       </c>
       <c r="D146" t="s">
         <v>506</v>
+      </c>
+      <c r="E146" t="s">
+        <v>51</v>
       </c>
       <c r="F146" t="s">
         <v>507</v>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-07-24 22:37:33
Affected files:
obsidian/Obsidian Share Vault/Friends and Family/Dad/Cognitive and Physical Training For Dad.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Obsidian Share Vault/lit/lit_notes/Ribeiro25resistTrainProtectMildCog.md
obsidian/Test Vault/.obsidian/app.json
obsidian/Test Vault/.obsidian/appearance.json
obsidian/Test Vault/.obsidian/community-plugins.json
obsidian/Test Vault/.obsidian/core-plugins.json
obsidian/Test Vault/.obsidian/workspace.json
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1171" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D4E657-94F6-47EB-9E86-9CC6418DEF29}"/>
+  <xr:revisionPtr revIDLastSave="1172" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6C8C4EA-C0C9-45F4-8036-FA5793AAFFC3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="34560" windowHeight="18996" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="514">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4959,28 +4959,28 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F146" sqref="F146"/>
+      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" customWidth="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1"/>
-    <col min="3" max="3" width="29.19921875" customWidth="1"/>
-    <col min="4" max="4" width="46.796875" customWidth="1"/>
-    <col min="5" max="5" width="8.53125" customWidth="1"/>
-    <col min="6" max="6" width="28.19921875" customWidth="1"/>
-    <col min="7" max="7" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45523</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45525</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>45528</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>45530</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>45531</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>45534</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>45539</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45539</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>45539</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>45540</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>45541</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>45541</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>45543</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>45547</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>45548</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>45549</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>45555</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>45555</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>45555</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>45555</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>45562</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>45563</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>45563</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>45563</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>45563</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45563</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>45563</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>45566</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>45569</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>45570</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>45577</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>45577</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>45577</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>45591</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>45591</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>45591</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>45595</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>45598</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>45598</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>45600</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>45600</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>45605</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45612</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>45612</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>45612</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>45616</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>45619</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>45619</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>45619</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>45626</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>45626</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>45626</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>45633</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>45633</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>45633</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>45635</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>45640</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>45640</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>45640</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>45641</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>45647</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>45647</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>45647</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>45647</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>45651</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>45651</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>45654</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>45654</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>45654</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>45661</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>45661</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>45661</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>45667</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>45668</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>45668</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>45668</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>45668</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>45674</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>45674</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>45675</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>45682</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>45682</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>45682</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>45682</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>45316</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>45688</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>45689</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>45689</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>45689</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>45696</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>45696</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>45696</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>45696</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>45703</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>45703</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>45703</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>45703</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>45708</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>45710</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>377</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>45717</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>45717</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>45717</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>45717</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>394</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>45723</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>45724</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>45731</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>45731</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>45731</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>45731</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>45731</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>45731</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>45731</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>45739</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>45739</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>45739</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>45740</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>45741</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>45746</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>45748</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>45770</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>45777</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>45772</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>45774</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>46878</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>45782</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>45782</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>45782</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>45784</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>45818</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>45818</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>45818</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>45818</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>45818</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>45818</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>45842</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>45842</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>45842</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>45842</v>
       </c>
@@ -7567,11 +7567,14 @@
       <c r="D144" t="s">
         <v>500</v>
       </c>
+      <c r="E144" t="s">
+        <v>51</v>
+      </c>
       <c r="F144" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>45842</v>
       </c>
@@ -7588,7 +7591,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>45481</v>
       </c>
@@ -7608,7 +7611,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>45846</v>
       </c>
@@ -7625,7 +7628,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>45846</v>
       </c>
@@ -7671,22 +7674,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -7706,7 +7709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7720,7 +7723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7757,7 +7760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7774,7 +7777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7791,7 +7794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7805,7 +7808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -7822,7 +7825,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45539</v>
       </c>
@@ -7842,7 +7845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45539</v>
       </c>
@@ -7859,7 +7862,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45539</v>
       </c>
@@ -7876,7 +7879,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45540</v>
       </c>
@@ -7896,7 +7899,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45541</v>
       </c>
@@ -7913,7 +7916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45541</v>
       </c>
@@ -7933,7 +7936,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45543</v>
       </c>
@@ -7953,7 +7956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45547</v>
       </c>
@@ -7970,7 +7973,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="3">
         <v>45548</v>
       </c>
@@ -7987,7 +7990,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C23" s="3">
         <v>45549</v>
       </c>
@@ -8004,7 +8007,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C24" s="3">
         <v>45555</v>
       </c>
@@ -8024,7 +8027,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C25" s="3">
         <v>45555</v>
       </c>
@@ -8041,7 +8044,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>45555</v>
       </c>
@@ -8058,7 +8061,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" s="3">
         <v>45555</v>
       </c>
@@ -8075,7 +8078,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>82</v>
       </c>
@@ -8092,7 +8095,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" s="3">
         <v>45563</v>
       </c>
@@ -8109,7 +8112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>45563</v>
       </c>
@@ -8126,7 +8129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
         <v>45563</v>
       </c>
@@ -8143,7 +8146,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>45563</v>
       </c>
@@ -8160,7 +8163,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C33" s="3">
         <v>45563</v>
       </c>
@@ -8177,7 +8180,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
         <v>45563</v>
       </c>
@@ -8205,23 +8208,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C5" cm="1">
         <f t="array" ref="C5">IF(SUM(ISERROR(Sheet2!$C$7:$H$34)*1)&gt;0,NA(),COUNTA(_xlfn.UNIQUE(Sheet2!$C$7:$C$34)))</f>
         <v>17</v>
@@ -8238,19 +8241,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -8258,7 +8261,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -8266,7 +8269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -8274,7 +8277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -8282,7 +8285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -8290,7 +8293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -8298,7 +8301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -8306,7 +8309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -8314,7 +8317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -8322,7 +8325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -8330,7 +8333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -8338,7 +8341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -8346,7 +8349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -8354,7 +8357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -8362,7 +8365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -8370,7 +8373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -8378,7 +8381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -8386,7 +8389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -8394,7 +8397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>119</v>
       </c>
@@ -8414,19 +8417,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.53125" customWidth="1"/>
-    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -8434,7 +8437,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -8442,7 +8445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -8450,7 +8453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -8458,7 +8461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -8466,7 +8469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -8474,7 +8477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -8482,7 +8485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -8490,7 +8493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -8498,7 +8501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -8506,7 +8509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -8514,7 +8517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -8522,7 +8525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -8530,7 +8533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -8538,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -8546,7 +8549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -8554,7 +8557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -8562,7 +8565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -8570,7 +8573,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-07-25 15:38:19
Affected files:
obsidian/Obsidian Share Vault/Friends and Family/Dad/Cognitive and Physical Training For Dad.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
obsidian/Test Vault/.obsidian/plugins/multi-properties/main.js
obsidian/Test Vault/.obsidian/plugins/multi-properties/manifest.json
obsidian/Test Vault/.obsidian/plugins/multi-properties/styles.css
obsidian/Test Vault/.obsidian/plugins/obsidian-multi-tab/main.js
obsidian/Test Vault/.obsidian/plugins/obsidian-multi-tab/manifest.json
obsidian/Test Vault/.obsidian/plugins/obsidian-multi-tab/styles.css
obsidian/Test Vault/MANUAL-TESTING-GUIDE.md
obsidian/Test Vault/test-note.md
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1172" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6C8C4EA-C0C9-45F4-8036-FA5793AAFFC3}"/>
+  <xr:revisionPtr revIDLastSave="1173" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{606E6BE4-F1FD-43B5-9E16-02388BEDCF77}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="34560" windowHeight="18996" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="514">
   <si>
     <t>Employment actions</t>
   </si>
@@ -4959,28 +4959,28 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G157" sqref="G157"/>
+      <selection pane="bottomLeft" activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="29.19921875" customWidth="1"/>
+    <col min="4" max="4" width="46.796875" customWidth="1"/>
+    <col min="5" max="5" width="8.53125" customWidth="1"/>
+    <col min="6" max="6" width="28.19921875" customWidth="1"/>
+    <col min="7" max="7" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>45523</v>
       </c>
@@ -5014,7 +5014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>45525</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>45528</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>45530</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>45531</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>45534</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>45539</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
         <v>45539</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>45539</v>
       </c>
@@ -5171,7 +5171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="3">
         <v>45540</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>45541</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="3">
         <v>45541</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>45543</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="3">
         <v>45547</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>45548</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="3">
         <v>45549</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>45555</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="3">
         <v>45555</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>45555</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="3">
         <v>45555</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="3">
         <v>45562</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="3">
         <v>45563</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="3">
         <v>45563</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="3">
         <v>45563</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
         <v>45563</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="3">
         <v>45563</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="3">
         <v>45563</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="3">
         <v>45566</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="3">
         <v>45569</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="3">
         <v>45570</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="13">
         <v>45577</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="3">
         <v>45577</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="3">
         <v>45577</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="3">
         <v>45591</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="3">
         <v>45591</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="3">
         <v>45591</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="3">
         <v>45595</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="3">
         <v>45598</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="3">
         <v>45598</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="3">
         <v>45600</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="3">
         <v>45600</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="3">
         <v>45605</v>
       </c>
@@ -5771,7 +5771,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="3">
         <v>45612</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="3">
         <v>45612</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="3">
         <v>45612</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="13">
         <v>45616</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="3">
         <v>45619</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="3">
         <v>45619</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="3">
         <v>45619</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="3">
         <v>45626</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="3">
         <v>45626</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="3">
         <v>45626</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="3">
         <v>45633</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="3">
         <v>45633</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>45633</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>45635</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>45640</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="3">
         <v>45640</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="3">
         <v>45640</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="3">
         <v>45641</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="3">
         <v>45647</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="3">
         <v>45647</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="3">
         <v>45647</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="3">
         <v>45647</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="3">
         <v>45651</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="3">
         <v>45651</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="3">
         <v>45654</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="3">
         <v>45654</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="3">
         <v>45654</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="3">
         <v>45661</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="3">
         <v>45661</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="3">
         <v>45661</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="3">
         <v>45667</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="3">
         <v>45668</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="3">
         <v>45668</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="3">
         <v>45668</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="3">
         <v>45668</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="3">
         <v>45674</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="3">
         <v>45674</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="3">
         <v>45675</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="3">
         <v>45682</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="3">
         <v>45682</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="3">
         <v>45682</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="3">
         <v>45682</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="3">
         <v>45316</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="3">
         <v>45688</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="3">
         <v>45689</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="3">
         <v>45689</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="3">
         <v>45689</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="3">
         <v>45696</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="3">
         <v>45696</v>
       </c>
@@ -6702,7 +6702,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="3">
         <v>45696</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="3">
         <v>45696</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A98" s="3">
         <v>45703</v>
       </c>
@@ -6756,7 +6756,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A99" s="3">
         <v>45703</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A100" s="3">
         <v>45703</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A101" s="3">
         <v>45703</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A102" s="3">
         <v>45708</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A103" s="3">
         <v>45710</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>377</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A105" s="3">
         <v>45717</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A106" s="3">
         <v>45717</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A107" s="3">
         <v>45717</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A108" s="3">
         <v>45717</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>394</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A110" s="3">
         <v>45723</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="3">
         <v>45724</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" s="3">
         <v>45731</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="3">
         <v>45731</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="3">
         <v>45731</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="3">
         <v>45731</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="3">
         <v>45731</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="3">
         <v>45731</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="3">
         <v>45731</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="3">
         <v>45739</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="3">
         <v>45739</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="3">
         <v>45739</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="3">
         <v>45740</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="3">
         <v>45741</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="3">
         <v>45746</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="3">
         <v>45748</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A126" s="3">
         <v>45770</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="3">
         <v>45777</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" s="3">
         <v>45772</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="3">
         <v>45774</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="3">
         <v>46878</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="3">
         <v>45782</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" s="3">
         <v>45782</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" s="3">
         <v>45782</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" s="3">
         <v>45784</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" s="3">
         <v>45818</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" s="3">
         <v>45818</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" s="3">
         <v>45818</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" s="3">
         <v>45818</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" s="3">
         <v>45818</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" s="3">
         <v>45818</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" s="3">
         <v>45842</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" s="3">
         <v>45842</v>
       </c>
@@ -7533,11 +7533,14 @@
       <c r="D142" t="s">
         <v>493</v>
       </c>
+      <c r="E142" t="s">
+        <v>51</v>
+      </c>
       <c r="F142" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" s="3">
         <v>45842</v>
       </c>
@@ -7554,7 +7557,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" s="3">
         <v>45842</v>
       </c>
@@ -7574,7 +7577,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="3">
         <v>45842</v>
       </c>
@@ -7591,7 +7594,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="3">
         <v>45481</v>
       </c>
@@ -7611,7 +7614,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" s="3">
         <v>45846</v>
       </c>
@@ -7628,7 +7631,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" s="3">
         <v>45846</v>
       </c>
@@ -7674,22 +7677,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B4" s="9"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -7709,7 +7712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -7723,7 +7726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -7740,7 +7743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -7760,7 +7763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -7777,7 +7780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -7794,7 +7797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -7808,7 +7811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -7825,7 +7828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45539</v>
       </c>
@@ -7845,7 +7848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45539</v>
       </c>
@@ -7862,7 +7865,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45539</v>
       </c>
@@ -7879,7 +7882,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45540</v>
       </c>
@@ -7899,7 +7902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45541</v>
       </c>
@@ -7916,7 +7919,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45541</v>
       </c>
@@ -7936,7 +7939,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45543</v>
       </c>
@@ -7956,7 +7959,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45547</v>
       </c>
@@ -7973,7 +7976,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C22" s="3">
         <v>45548</v>
       </c>
@@ -7990,7 +7993,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C23" s="3">
         <v>45549</v>
       </c>
@@ -8007,7 +8010,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C24" s="3">
         <v>45555</v>
       </c>
@@ -8027,7 +8030,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C25" s="3">
         <v>45555</v>
       </c>
@@ -8044,7 +8047,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C26" s="3">
         <v>45555</v>
       </c>
@@ -8061,7 +8064,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C27" s="3">
         <v>45555</v>
       </c>
@@ -8078,7 +8081,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>82</v>
       </c>
@@ -8095,7 +8098,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C29" s="3">
         <v>45563</v>
       </c>
@@ -8112,7 +8115,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C30" s="3">
         <v>45563</v>
       </c>
@@ -8129,7 +8132,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C31" s="3">
         <v>45563</v>
       </c>
@@ -8146,7 +8149,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C32" s="3">
         <v>45563</v>
       </c>
@@ -8163,7 +8166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C33" s="3">
         <v>45563</v>
       </c>
@@ -8180,7 +8183,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C34" s="3">
         <v>45563</v>
       </c>
@@ -8208,23 +8211,23 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C4" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C5" cm="1">
         <f t="array" ref="C5">IF(SUM(ISERROR(Sheet2!$C$7:$H$34)*1)&gt;0,NA(),COUNTA(_xlfn.UNIQUE(Sheet2!$C$7:$C$34)))</f>
         <v>17</v>
@@ -8241,19 +8244,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -8261,7 +8264,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -8269,7 +8272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -8277,7 +8280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -8285,7 +8288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -8293,7 +8296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -8301,7 +8304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -8309,7 +8312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -8317,7 +8320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -8325,7 +8328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -8333,7 +8336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -8341,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -8349,7 +8352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -8357,7 +8360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -8365,7 +8368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -8373,7 +8376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -8381,7 +8384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -8389,7 +8392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -8397,7 +8400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>119</v>
       </c>
@@ -8417,19 +8420,19 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="3.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.53125" customWidth="1"/>
+    <col min="3" max="3" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
@@ -8437,7 +8440,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -8445,7 +8448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>82</v>
       </c>
@@ -8453,7 +8456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C7" s="3">
         <v>45523</v>
       </c>
@@ -8461,7 +8464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C8" s="3">
         <v>45525</v>
       </c>
@@ -8469,7 +8472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C9" s="3">
         <v>45528</v>
       </c>
@@ -8477,7 +8480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C10" s="3">
         <v>45530</v>
       </c>
@@ -8485,7 +8488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C11" s="3">
         <v>45531</v>
       </c>
@@ -8493,7 +8496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="3">
         <v>45534</v>
       </c>
@@ -8501,7 +8504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C13" s="3">
         <v>45539</v>
       </c>
@@ -8509,7 +8512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C14" s="3">
         <v>45540</v>
       </c>
@@ -8517,7 +8520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C15" s="3">
         <v>45541</v>
       </c>
@@ -8525,7 +8528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C16" s="3">
         <v>45543</v>
       </c>
@@ -8533,7 +8536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C17" s="3">
         <v>45547</v>
       </c>
@@ -8541,7 +8544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C18" s="3">
         <v>45548</v>
       </c>
@@ -8549,7 +8552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C19" s="3">
         <v>45549</v>
       </c>
@@ -8557,7 +8560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C20" s="3">
         <v>45555</v>
       </c>
@@ -8565,7 +8568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C21" s="3">
         <v>45563</v>
       </c>
@@ -8573,7 +8576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>119</v>
       </c>

</xml_diff>

<commit_message>
obsidian backup auto: 2025-07-31 14:22:13
Affected files:
.emacs
.gitignore
obsidian/Obsidian Share Vault/Evernote to Obsidian and Zotero.md
obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
</commit_message>
<xml_diff>
--- a/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
+++ b/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/jobactions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4BBD96B3698748F8/share/ref/obsidian/Obsidian Share Vault/Work/Between Jobs/QCELLs offboarding/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1173" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{606E6BE4-F1FD-43B5-9E16-02388BEDCF77}"/>
+  <xr:revisionPtr revIDLastSave="1187" documentId="8_{CE52EC3F-5AF1-405A-AFA1-BE79F5966B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE5C9DCE-E5EB-4D01-99A3-D0601625C936}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="10522" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
+    <workbookView minimized="1" xWindow="-19395" yWindow="4050" windowWidth="16200" windowHeight="10523" xr2:uid="{F4947C1B-4D46-46A7-B94B-4FA0E1485E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="519">
   <si>
     <t>Employment actions</t>
   </si>
@@ -1607,6 +1607,21 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/4260947802/?refId=ByteString(length%3D16%2Cbytes%3Da8c5a42f...11bc97f5)&amp;trackingId=b9wobbPUJfn7ROl96c7mFQ%3D%3D</t>
+  </si>
+  <si>
+    <t>Data Scientist - Fiber</t>
+  </si>
+  <si>
+    <t>https://careers.t-mobile.com/data-scientist-fiber-team/job/BF64F9A308F7B1AC2713CE5CA27444D5?source=LinkedIn&amp;codes=INT-LinkedIn</t>
+  </si>
+  <si>
+    <t>Acubed by Airbus</t>
+  </si>
+  <si>
+    <t>I got a linked in message from Bix Cruz, an Airbus recruiter</t>
+  </si>
+  <si>
+    <t>https://mail.google.com/mail/u/0/#inbox/FMfcgzQbgcLsdgrzkXDwgkRkRhzFVwJJ</t>
   </si>
 </sst>
 </file>
@@ -4955,11 +4970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9800ADB-CF3C-401A-B566-2EB8777B4132}">
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7646,6 +7661,40 @@
       </c>
       <c r="F148" s="5" t="s">
         <v>513</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A149" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B149" t="s">
+        <v>256</v>
+      </c>
+      <c r="C149" t="s">
+        <v>514</v>
+      </c>
+      <c r="D149" t="s">
+        <v>172</v>
+      </c>
+      <c r="F149" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A150" s="3">
+        <v>45868</v>
+      </c>
+      <c r="B150" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="C150" t="s">
+        <v>79</v>
+      </c>
+      <c r="D150" t="s">
+        <v>517</v>
+      </c>
+      <c r="F150" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>